<commit_message>
Configuration update after IOS 2015
</commit_message>
<xml_diff>
--- a/RBCC_E/configs/icf157.xlsx
+++ b/RBCC_E/configs/icf157.xlsx
@@ -1547,7 +1547,7 @@
   <dimension ref="A1:AY54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AY2" sqref="AY2"/>
+      <selection activeCell="AW26" sqref="AW26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5623,13 +5623,13 @@
         <v>1</v>
       </c>
       <c r="AW26" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX26" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY26" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:51">

</xml_diff>

<commit_message>
introducidos datos en la blacklist
</commit_message>
<xml_diff>
--- a/RBCC_E/configs/icf157.xlsx
+++ b/RBCC_E/configs/icf157.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
-  <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr showInkAnnotation="0" codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODE\iberonesia\RBCC_E\configs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="820" yWindow="0" windowWidth="25480" windowHeight="26000" activeTab="2"/>
+    <workbookView xWindow="825" yWindow="465" windowWidth="25605" windowHeight="11880" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="icf.157" sheetId="1" r:id="rId1"/>
@@ -13,11 +18,12 @@
     <sheet name="Incidencias.157" sheetId="3" r:id="rId4"/>
     <sheet name="DV-IDENTITY-0" sheetId="4" state="veryHidden" r:id="rId5"/>
     <sheet name="Cfg_reduced" sheetId="11" r:id="rId6"/>
+    <sheet name="blacklist.157" sheetId="12" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="cfg_s157" localSheetId="5">Cfg_reduced!$C$1:$X$54</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -61,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="220">
   <si>
     <t>#</t>
   </si>
@@ -679,21 +685,6 @@
     <t>"IOS15"</t>
   </si>
   <si>
-    <t>Calibración 1000W</t>
-  </si>
-  <si>
-    <t>Brewer retirado temporal</t>
-  </si>
-  <si>
-    <t>Manteniemiento Kipp&amp;Zonen</t>
-  </si>
-  <si>
-    <t>Brewer parado por cambio cuadro eléctrico</t>
-  </si>
-  <si>
-    <t>Brewer bajado para calibración de 1000W</t>
-  </si>
-  <si>
     <t>icf16014.158</t>
   </si>
   <si>
@@ -706,7 +697,37 @@
     <t>icf16014.162</t>
   </si>
   <si>
-    <t>Brewercalibración de 1000W</t>
+    <t>"Cal. 1000W"</t>
+  </si>
+  <si>
+    <t>"Brewer bad weather"</t>
+  </si>
+  <si>
+    <t>" Kipp&amp;Zonen"</t>
+  </si>
+  <si>
+    <t>"Cal 1000W"</t>
+  </si>
+  <si>
+    <t>IOS15</t>
+  </si>
+  <si>
+    <t>Calib.1000W</t>
+  </si>
+  <si>
+    <t>Brewer bad weather</t>
+  </si>
+  <si>
+    <t>Kipp&amp;Zonen</t>
+  </si>
+  <si>
+    <t>Cal. 1000W</t>
+  </si>
+  <si>
+    <t>Change electric system</t>
+  </si>
+  <si>
+    <t>Wrong data for lower sza, sighting</t>
   </si>
 </sst>
 </file>
@@ -714,9 +735,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -742,69 +763,10 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Cambria"/>
-      <family val="2"/>
-      <scheme val="major"/>
     </font>
     <font>
       <b/>
@@ -821,153 +783,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="30">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="31"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="45"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="46"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="36"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="52"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -981,51 +809,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1040,42 +829,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1092,13 +851,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1117,7 +876,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1143,45 +902,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="33">
-    <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="2" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="3" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="4" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="5" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="6" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="7" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="8" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="9" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="10" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="11" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="12" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="13" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="14" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="15" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="16" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="17" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="18" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="19" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="20" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="21" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="23" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="24" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="25" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="26" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="27" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorrecto" xfId="28" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="3">
+    <cellStyle name="Neutral" xfId="1" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Salida" xfId="30" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="31" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="32" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="2" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1253,6 +983,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1582,21 +1320,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:BD54"/>
   <sheetViews>
-    <sheetView topLeftCell="AT1" workbookViewId="0">
-      <selection activeCell="BD3" sqref="BD3"/>
+    <sheetView showRuler="0" topLeftCell="AS9" workbookViewId="0">
+      <selection activeCell="BD13" sqref="BD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="10"/>
-    <col min="2" max="2" width="29.1640625" style="7" customWidth="1"/>
-    <col min="3" max="16384" width="11.33203125" style="13"/>
+    <col min="1" max="1" width="11.28515625" style="10"/>
+    <col min="2" max="2" width="29.140625" style="7" customWidth="1"/>
+    <col min="3" max="16384" width="11.28515625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" s="8" customFormat="1">
+    <row r="1" spans="1:56" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="8">
@@ -1811,7 +1549,7 @@
         <v>42446</v>
       </c>
     </row>
-    <row r="2" spans="1:56" s="10" customFormat="1">
+    <row r="2" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1981,7 +1719,7 @@
         <v>736406</v>
       </c>
     </row>
-    <row r="3" spans="1:56" ht="18" customHeight="1">
+    <row r="3" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -2151,7 +1889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:56">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -2321,7 +2059,7 @@
         <v>-0.17899999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:56">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -2491,7 +2229,7 @@
         <v>-0.33350000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:56">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -2661,7 +2399,7 @@
         <v>-0.21299999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:56">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -2831,7 +2569,7 @@
         <v>-0.5645</v>
       </c>
     </row>
-    <row r="8" spans="1:56">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -3001,7 +2739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:56">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -3171,7 +2909,7 @@
         <v>0.33950000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:56">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -3341,7 +3079,7 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="11" spans="1:56">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -3511,7 +3249,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:56" s="10" customFormat="1" ht="17.25" customHeight="1">
+    <row r="12" spans="1:56" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -3663,25 +3401,25 @@
         <v>1580</v>
       </c>
       <c r="AY12" s="7">
-        <v>1580</v>
+        <v>1590</v>
       </c>
       <c r="AZ12" s="7">
-        <v>1580</v>
+        <v>1590</v>
       </c>
       <c r="BA12" s="7">
-        <v>1580</v>
+        <v>1590</v>
       </c>
       <c r="BB12" s="7">
-        <v>1580</v>
+        <v>1590</v>
       </c>
       <c r="BC12" s="7">
-        <v>1580</v>
+        <v>1590</v>
       </c>
       <c r="BD12" s="7">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="13" spans="1:56" s="10" customFormat="1">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="13" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -3851,7 +3589,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="1:56" s="17" customFormat="1" ht="17.25" customHeight="1">
+    <row r="14" spans="1:56" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>12</v>
       </c>
@@ -4021,7 +3759,7 @@
         <v>2.7999999999999999E-8</v>
       </c>
     </row>
-    <row r="15" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1">
+    <row r="15" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -4191,7 +3929,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="16" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1">
+    <row r="16" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -4361,7 +4099,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1">
+    <row r="17" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>15</v>
       </c>
@@ -4531,7 +4269,7 @@
         <v>2439</v>
       </c>
     </row>
-    <row r="18" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="18" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>16</v>
       </c>
@@ -4701,7 +4439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="19" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>17</v>
       </c>
@@ -4871,7 +4609,7 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="20" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="20" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>18</v>
       </c>
@@ -5041,7 +4779,7 @@
         <v>9320</v>
       </c>
     </row>
-    <row r="21" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="21" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>19</v>
       </c>
@@ -5211,7 +4949,7 @@
         <v>13860</v>
       </c>
     </row>
-    <row r="22" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="22" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>20</v>
       </c>
@@ -5381,7 +5119,7 @@
         <v>21660</v>
       </c>
     </row>
-    <row r="23" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="23" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>21</v>
       </c>
@@ -5551,7 +5289,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="24" spans="1:56" s="10" customFormat="1">
+    <row r="24" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>22</v>
       </c>
@@ -5721,7 +5459,7 @@
         <v>2972</v>
       </c>
     </row>
-    <row r="25" spans="1:56" s="10" customFormat="1">
+    <row r="25" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>23</v>
       </c>
@@ -5891,7 +5629,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:56" s="10" customFormat="1">
+    <row r="26" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>24</v>
       </c>
@@ -6061,7 +5799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:56">
+    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>25</v>
       </c>
@@ -6231,7 +5969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:56">
+    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>26</v>
       </c>
@@ -6401,7 +6139,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="29" spans="1:56">
+    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>27</v>
       </c>
@@ -6571,7 +6309,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="30" spans="1:56">
+    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>28</v>
       </c>
@@ -6741,7 +6479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:56">
+    <row r="31" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>29</v>
       </c>
@@ -6911,7 +6649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:56">
+    <row r="32" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>30</v>
       </c>
@@ -7081,7 +6819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:56">
+    <row r="33" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>31</v>
       </c>
@@ -7251,7 +6989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:56">
+    <row r="34" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>32</v>
       </c>
@@ -7421,7 +7159,7 @@
         <v>7420</v>
       </c>
     </row>
-    <row r="35" spans="1:56" s="10" customFormat="1">
+    <row r="35" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>33</v>
       </c>
@@ -7591,7 +7329,7 @@
         <v>6025</v>
       </c>
     </row>
-    <row r="36" spans="1:56" s="10" customFormat="1">
+    <row r="36" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>34</v>
       </c>
@@ -7761,7 +7499,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="37" spans="1:56" s="10" customFormat="1">
+    <row r="37" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>35</v>
       </c>
@@ -7931,7 +7669,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="1:56" s="10" customFormat="1">
+    <row r="38" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>36</v>
       </c>
@@ -8101,7 +7839,7 @@
         <v>67397790</v>
       </c>
     </row>
-    <row r="39" spans="1:56" s="10" customFormat="1">
+    <row r="39" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>37</v>
       </c>
@@ -8271,7 +8009,7 @@
         <v>54644647</v>
       </c>
     </row>
-    <row r="40" spans="1:56" s="10" customFormat="1">
+    <row r="40" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>38</v>
       </c>
@@ -8441,7 +8179,7 @@
         <v>88722733</v>
       </c>
     </row>
-    <row r="41" spans="1:56" s="10" customFormat="1">
+    <row r="41" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>39</v>
       </c>
@@ -8611,7 +8349,7 @@
         <v>92846918</v>
       </c>
     </row>
-    <row r="42" spans="1:56" s="10" customFormat="1">
+    <row r="42" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>40</v>
       </c>
@@ -8781,7 +8519,7 @@
         <v>100533789</v>
       </c>
     </row>
-    <row r="43" spans="1:56">
+    <row r="43" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>41</v>
       </c>
@@ -8951,7 +8689,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="44" spans="1:56">
+    <row r="44" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>42</v>
       </c>
@@ -9121,7 +8859,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="45" spans="1:56" s="10" customFormat="1" ht="11.25" customHeight="1">
+    <row r="45" spans="1:56" s="10" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>43</v>
       </c>
@@ -9291,7 +9029,7 @@
         <v>1732</v>
       </c>
     </row>
-    <row r="46" spans="1:56" s="10" customFormat="1">
+    <row r="46" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>44</v>
       </c>
@@ -9461,7 +9199,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="47" spans="1:56" s="10" customFormat="1">
+    <row r="47" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>45</v>
       </c>
@@ -9631,7 +9369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:56" s="10" customFormat="1">
+    <row r="48" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>46</v>
       </c>
@@ -9801,7 +9539,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:56" s="10" customFormat="1">
+    <row r="49" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>47</v>
       </c>
@@ -9971,7 +9709,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="50" spans="1:56" s="10" customFormat="1">
+    <row r="50" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>48</v>
       </c>
@@ -10141,7 +9879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:56" s="10" customFormat="1">
+    <row r="51" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>49</v>
       </c>
@@ -10311,7 +10049,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:56" s="10" customFormat="1">
+    <row r="52" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>50</v>
       </c>
@@ -10481,7 +10219,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:56" s="10" customFormat="1">
+    <row r="53" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>51</v>
       </c>
@@ -10651,7 +10389,7 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="54" spans="1:56">
+    <row r="54" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>52</v>
       </c>
@@ -10674,30 +10412,25 @@
   <customProperties>
     <customPr name="DVSECTIONID" r:id="rId1"/>
   </customProperties>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BD54"/>
+  <dimension ref="A1:BF54"/>
   <sheetViews>
-    <sheetView topLeftCell="AT1" workbookViewId="0">
-      <selection activeCell="BD4" sqref="BD4"/>
+    <sheetView showRuler="0" topLeftCell="AP14" workbookViewId="0">
+      <selection activeCell="BD29" sqref="BD29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="10"/>
-    <col min="2" max="2" width="29.1640625" style="7" customWidth="1"/>
-    <col min="3" max="16384" width="11.33203125" style="13"/>
+    <col min="1" max="1" width="11.28515625" style="10"/>
+    <col min="2" max="2" width="29.140625" style="7" customWidth="1"/>
+    <col min="3" max="16384" width="11.28515625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" s="8" customFormat="1">
+    <row r="1" spans="1:58" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="8">
@@ -10912,7 +10645,7 @@
         <v>42446</v>
       </c>
     </row>
-    <row r="2" spans="1:56" s="10" customFormat="1">
+    <row r="2" spans="1:58" s="10" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -11081,8 +10814,9 @@
       <c r="BD2" s="4">
         <v>736406</v>
       </c>
-    </row>
-    <row r="3" spans="1:56" ht="18" customHeight="1">
+      <c r="BF2" s="39"/>
+    </row>
+    <row r="3" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -11234,25 +10968,25 @@
         <v>0</v>
       </c>
       <c r="AY3" s="14">
-        <v>0</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="AZ3" s="14">
-        <v>0</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="BA3" s="14">
-        <v>0</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="BB3" s="14">
-        <v>0</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="BC3" s="14">
-        <v>0</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="BD3" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:56">
+        <v>-1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -11404,25 +11138,25 @@
         <v>-0.17899999999999999</v>
       </c>
       <c r="AY4" s="14">
-        <v>-0.17899999999999999</v>
+        <v>-0.6</v>
       </c>
       <c r="AZ4" s="14">
-        <v>-0.17899999999999999</v>
+        <v>-0.6</v>
       </c>
       <c r="BA4" s="14">
-        <v>-0.17899999999999999</v>
+        <v>-0.6</v>
       </c>
       <c r="BB4" s="14">
-        <v>-0.17899999999999999</v>
+        <v>-0.6</v>
       </c>
       <c r="BC4" s="14">
-        <v>-0.17899999999999999</v>
+        <v>-0.6</v>
       </c>
       <c r="BD4" s="14">
-        <v>-0.17899999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:56">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -11574,25 +11308,25 @@
         <v>-0.33350000000000002</v>
       </c>
       <c r="AY5" s="14">
-        <v>-0.33350000000000002</v>
+        <v>0</v>
       </c>
       <c r="AZ5" s="14">
-        <v>-0.33350000000000002</v>
+        <v>0</v>
       </c>
       <c r="BA5" s="14">
-        <v>-0.33350000000000002</v>
+        <v>0</v>
       </c>
       <c r="BB5" s="14">
-        <v>-0.33350000000000002</v>
+        <v>0</v>
       </c>
       <c r="BC5" s="14">
-        <v>-0.33350000000000002</v>
+        <v>0</v>
       </c>
       <c r="BD5" s="14">
-        <v>-0.33350000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -11744,25 +11478,25 @@
         <v>-0.21299999999999999</v>
       </c>
       <c r="AY6" s="14">
-        <v>-0.21299999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="AZ6" s="14">
-        <v>-0.21299999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="BA6" s="14">
-        <v>-0.21299999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="BB6" s="14">
-        <v>-0.21299999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="BC6" s="14">
-        <v>-0.21299999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="BD6" s="14">
-        <v>-0.21299999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:56">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -11914,25 +11648,25 @@
         <v>-0.5645</v>
       </c>
       <c r="AY7" s="14">
-        <v>-0.5645</v>
+        <v>0</v>
       </c>
       <c r="AZ7" s="14">
-        <v>-0.5645</v>
+        <v>0</v>
       </c>
       <c r="BA7" s="14">
-        <v>-0.5645</v>
+        <v>0</v>
       </c>
       <c r="BB7" s="14">
-        <v>-0.5645</v>
+        <v>0</v>
       </c>
       <c r="BC7" s="14">
-        <v>-0.5645</v>
+        <v>0</v>
       </c>
       <c r="BD7" s="14">
-        <v>-0.5645</v>
-      </c>
-    </row>
-    <row r="8" spans="1:56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -12102,7 +11836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:56">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -12272,7 +12006,7 @@
         <v>0.33950000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:56">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -12442,7 +12176,7 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="11" spans="1:56">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -12612,7 +12346,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:56" s="10" customFormat="1" ht="17.25" customHeight="1">
+    <row r="12" spans="1:58" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -12764,25 +12498,25 @@
         <v>1580</v>
       </c>
       <c r="AY12" s="7">
-        <v>1580</v>
+        <v>1610</v>
       </c>
       <c r="AZ12" s="7">
-        <v>1580</v>
+        <v>1610</v>
       </c>
       <c r="BA12" s="7">
-        <v>1580</v>
+        <v>1610</v>
       </c>
       <c r="BB12" s="7">
-        <v>1580</v>
+        <v>1610</v>
       </c>
       <c r="BC12" s="7">
-        <v>1580</v>
+        <v>1610</v>
       </c>
       <c r="BD12" s="7">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="13" spans="1:56" s="10" customFormat="1">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="13" spans="1:58" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -12952,7 +12686,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="1:56" s="17" customFormat="1" ht="17.25" customHeight="1">
+    <row r="14" spans="1:58" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>12</v>
       </c>
@@ -13122,7 +12856,7 @@
         <v>2.7999999999999999E-8</v>
       </c>
     </row>
-    <row r="15" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1">
+    <row r="15" spans="1:58" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -13292,7 +13026,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="16" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1">
+    <row r="16" spans="1:58" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -13462,7 +13196,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1">
+    <row r="17" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>15</v>
       </c>
@@ -13632,7 +13366,7 @@
         <v>2439</v>
       </c>
     </row>
-    <row r="18" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="18" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>16</v>
       </c>
@@ -13802,7 +13536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="19" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>17</v>
       </c>
@@ -13972,7 +13706,7 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="20" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="20" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>18</v>
       </c>
@@ -14142,7 +13876,7 @@
         <v>9320</v>
       </c>
     </row>
-    <row r="21" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="21" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>19</v>
       </c>
@@ -14312,7 +14046,7 @@
         <v>13860</v>
       </c>
     </row>
-    <row r="22" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="22" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>20</v>
       </c>
@@ -14482,7 +14216,7 @@
         <v>21660</v>
       </c>
     </row>
-    <row r="23" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="23" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>21</v>
       </c>
@@ -14652,7 +14386,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="24" spans="1:56" s="10" customFormat="1">
+    <row r="24" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>22</v>
       </c>
@@ -14822,7 +14556,7 @@
         <v>2972</v>
       </c>
     </row>
-    <row r="25" spans="1:56" s="10" customFormat="1">
+    <row r="25" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>23</v>
       </c>
@@ -14992,7 +14726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:56" s="10" customFormat="1">
+    <row r="26" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>24</v>
       </c>
@@ -15162,7 +14896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:56">
+    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>25</v>
       </c>
@@ -15332,7 +15066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:56">
+    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>26</v>
       </c>
@@ -15484,25 +15218,25 @@
         <v>342</v>
       </c>
       <c r="AY28" s="7">
-        <v>342</v>
+        <v>365</v>
       </c>
       <c r="AZ28" s="7">
-        <v>342</v>
+        <v>365</v>
       </c>
       <c r="BA28" s="7">
-        <v>342</v>
+        <v>365</v>
       </c>
       <c r="BB28" s="7">
-        <v>342</v>
+        <v>365</v>
       </c>
       <c r="BC28" s="7">
-        <v>342</v>
+        <v>365</v>
       </c>
       <c r="BD28" s="7">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="29" spans="1:56">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>27</v>
       </c>
@@ -15672,7 +15406,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="30" spans="1:56">
+    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>28</v>
       </c>
@@ -15842,7 +15576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:56">
+    <row r="31" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>29</v>
       </c>
@@ -16012,7 +15746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:56">
+    <row r="32" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>30</v>
       </c>
@@ -16182,7 +15916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:56">
+    <row r="33" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>31</v>
       </c>
@@ -16352,7 +16086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:56">
+    <row r="34" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>32</v>
       </c>
@@ -16522,7 +16256,7 @@
         <v>7420</v>
       </c>
     </row>
-    <row r="35" spans="1:56" s="10" customFormat="1">
+    <row r="35" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>33</v>
       </c>
@@ -16692,7 +16426,7 @@
         <v>6025</v>
       </c>
     </row>
-    <row r="36" spans="1:56" s="10" customFormat="1">
+    <row r="36" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>34</v>
       </c>
@@ -16862,7 +16596,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="37" spans="1:56" s="10" customFormat="1">
+    <row r="37" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>35</v>
       </c>
@@ -17032,7 +16766,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="1:56" s="10" customFormat="1">
+    <row r="38" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>36</v>
       </c>
@@ -17202,7 +16936,7 @@
         <v>67397790</v>
       </c>
     </row>
-    <row r="39" spans="1:56" s="10" customFormat="1">
+    <row r="39" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>37</v>
       </c>
@@ -17372,7 +17106,7 @@
         <v>54644647</v>
       </c>
     </row>
-    <row r="40" spans="1:56" s="10" customFormat="1">
+    <row r="40" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>38</v>
       </c>
@@ -17542,7 +17276,7 @@
         <v>88722733</v>
       </c>
     </row>
-    <row r="41" spans="1:56" s="10" customFormat="1">
+    <row r="41" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>39</v>
       </c>
@@ -17712,7 +17446,7 @@
         <v>92846918</v>
       </c>
     </row>
-    <row r="42" spans="1:56" s="10" customFormat="1">
+    <row r="42" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>40</v>
       </c>
@@ -17882,7 +17616,7 @@
         <v>100533789</v>
       </c>
     </row>
-    <row r="43" spans="1:56">
+    <row r="43" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>41</v>
       </c>
@@ -18052,7 +17786,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="44" spans="1:56">
+    <row r="44" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>42</v>
       </c>
@@ -18222,7 +17956,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="45" spans="1:56" s="10" customFormat="1" ht="11.25" customHeight="1">
+    <row r="45" spans="1:56" s="10" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>43</v>
       </c>
@@ -18392,7 +18126,7 @@
         <v>1732</v>
       </c>
     </row>
-    <row r="46" spans="1:56" s="10" customFormat="1">
+    <row r="46" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>44</v>
       </c>
@@ -18562,7 +18296,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="47" spans="1:56" s="10" customFormat="1">
+    <row r="47" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>45</v>
       </c>
@@ -18732,7 +18466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:56" s="10" customFormat="1">
+    <row r="48" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>46</v>
       </c>
@@ -18902,7 +18636,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:56" s="10" customFormat="1">
+    <row r="49" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>47</v>
       </c>
@@ -19072,7 +18806,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="50" spans="1:56" s="10" customFormat="1">
+    <row r="50" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>48</v>
       </c>
@@ -19242,7 +18976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:56" s="10" customFormat="1">
+    <row r="51" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>49</v>
       </c>
@@ -19412,7 +19146,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:56" s="10" customFormat="1">
+    <row r="52" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>50</v>
       </c>
@@ -19582,7 +19316,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:56" s="10" customFormat="1">
+    <row r="53" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>51</v>
       </c>
@@ -19752,7 +19486,7 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="54" spans="1:56">
+    <row r="54" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>52</v>
       </c>
@@ -19772,32 +19506,27 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja2" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView showRuler="0" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5">
         <f t="shared" ref="A1:A32" si="0">+B1-693960</f>
         <v>35431</v>
@@ -19815,7 +19544,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <f t="shared" si="0"/>
         <v>35945</v>
@@ -19833,7 +19562,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <f t="shared" si="0"/>
         <v>36409</v>
@@ -19851,7 +19580,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <f t="shared" si="0"/>
         <v>36682</v>
@@ -19869,7 +19598,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <f t="shared" si="0"/>
         <v>37149</v>
@@ -19887,7 +19616,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <f t="shared" si="0"/>
         <v>37507</v>
@@ -19905,7 +19634,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <f t="shared" si="0"/>
         <v>37877</v>
@@ -19923,7 +19652,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <f t="shared" si="0"/>
         <v>38245</v>
@@ -19941,7 +19670,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <f t="shared" si="0"/>
         <v>38503</v>
@@ -19956,7 +19685,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <f t="shared" si="0"/>
         <v>38615</v>
@@ -19974,7 +19703,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <f t="shared" si="0"/>
         <v>39000</v>
@@ -19992,7 +19721,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <f t="shared" si="0"/>
         <v>39320</v>
@@ -20010,7 +19739,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <f t="shared" si="0"/>
         <v>39981</v>
@@ -20028,7 +19757,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <f t="shared" si="0"/>
         <v>40017</v>
@@ -20046,7 +19775,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <f t="shared" si="0"/>
         <v>40024</v>
@@ -20064,7 +19793,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <f t="shared" si="0"/>
         <v>40060</v>
@@ -20082,7 +19811,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <f t="shared" si="0"/>
         <v>40176</v>
@@ -20100,7 +19829,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <f t="shared" si="0"/>
         <v>40238</v>
@@ -20118,7 +19847,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <f t="shared" si="0"/>
         <v>40267</v>
@@ -20136,7 +19865,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <f t="shared" si="0"/>
         <v>40351</v>
@@ -20154,7 +19883,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <f t="shared" si="0"/>
         <v>40445</v>
@@ -20172,7 +19901,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <f>+B22-693960</f>
         <v>40512</v>
@@ -20190,7 +19919,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <f>+B23-693960</f>
         <v>40571</v>
@@ -20208,7 +19937,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <f t="shared" si="0"/>
         <v>40602</v>
@@ -20226,7 +19955,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <f t="shared" si="0"/>
         <v>40646</v>
@@ -20244,7 +19973,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <f t="shared" si="0"/>
         <v>40681</v>
@@ -20262,7 +19991,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <f t="shared" si="0"/>
         <v>40703</v>
@@ -20280,7 +20009,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <f t="shared" si="0"/>
         <v>40742</v>
@@ -20298,7 +20027,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <f>+B29-693960</f>
         <v>40777</v>
@@ -20316,7 +20045,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <f>+B30-693960</f>
         <v>40780</v>
@@ -20334,7 +20063,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <f t="shared" si="0"/>
         <v>40855</v>
@@ -20352,7 +20081,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <f t="shared" si="0"/>
         <v>40919</v>
@@ -20370,7 +20099,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <f t="shared" ref="A33:A39" si="1">+B33-693960</f>
         <v>41157</v>
@@ -20388,7 +20117,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <f t="shared" si="1"/>
         <v>41206</v>
@@ -20406,7 +20135,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f t="shared" si="1"/>
         <v>41394</v>
@@ -20424,7 +20153,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <f t="shared" si="1"/>
         <v>41682</v>
@@ -20442,7 +20171,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f>+B37-693960</f>
         <v>41715</v>
@@ -20460,7 +20189,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f>+B38-693960</f>
         <v>41758</v>
@@ -20478,7 +20207,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f t="shared" si="1"/>
         <v>41773</v>
@@ -20496,7 +20225,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>41782</v>
       </c>
@@ -20513,9 +20242,9 @@
         <v>343</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="20">
-        <f t="shared" ref="A41:A47" si="2">+B41-693960</f>
+        <f t="shared" ref="A41:A54" si="2">+B41-693960</f>
         <v>41800</v>
       </c>
       <c r="B41" s="4">
@@ -20531,7 +20260,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="20">
         <f t="shared" si="2"/>
         <v>41897</v>
@@ -20549,7 +20278,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="7" customFormat="1">
+    <row r="43" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20">
         <f t="shared" si="2"/>
         <v>41991</v>
@@ -20567,7 +20296,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="7" customFormat="1">
+    <row r="44" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="20">
         <f t="shared" si="2"/>
         <v>42027</v>
@@ -20585,7 +20314,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="7" customFormat="1">
+    <row r="45" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="20">
         <f t="shared" si="2"/>
         <v>42080</v>
@@ -20603,7 +20332,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="7" customFormat="1">
+    <row r="46" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20">
         <f t="shared" si="2"/>
         <v>42104</v>
@@ -20621,8 +20350,8 @@
         <v>350</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="20">
         <f t="shared" si="2"/>
         <v>42109</v>
       </c>
@@ -20639,9 +20368,9 @@
         <v>350</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="5">
-        <f>+B48-693960</f>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="20">
+        <f t="shared" si="2"/>
         <v>42122</v>
       </c>
       <c r="B48" s="4">
@@ -20657,8 +20386,9 @@
         <v>350</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="20">
+        <f t="shared" si="2"/>
         <v>42161</v>
       </c>
       <c r="B49" s="4">
@@ -20674,15 +20404,16 @@
         <v>350</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="21">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="20">
+        <f t="shared" si="2"/>
         <v>42276</v>
       </c>
       <c r="B50" s="4">
-        <v>736348</v>
+        <v>736236</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="D50" t="s">
         <v>156</v>
@@ -20691,75 +20422,79 @@
         <v>350</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="21">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="20">
+        <f t="shared" si="2"/>
         <v>42388</v>
       </c>
       <c r="B51" s="4">
-        <v>736236</v>
+        <v>736348</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="D51" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E51">
         <v>350</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="21">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="20">
+        <f t="shared" si="2"/>
         <v>42417</v>
       </c>
       <c r="B52" s="4">
-        <v>736348</v>
+        <v>736377</v>
       </c>
       <c r="C52" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="D52" t="s">
         <v>206</v>
-      </c>
-      <c r="D52" t="s">
-        <v>211</v>
       </c>
       <c r="E52">
         <v>350</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="21">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="20">
+        <f t="shared" si="2"/>
         <v>42438</v>
       </c>
       <c r="B53" s="4">
-        <v>736377</v>
+        <v>736398</v>
       </c>
       <c r="C53" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="D53" t="s">
         <v>207</v>
-      </c>
-      <c r="D53" t="s">
-        <v>212</v>
       </c>
       <c r="E53">
         <v>350</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="21">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="20">
+        <f t="shared" si="2"/>
         <v>42446</v>
       </c>
       <c r="B54" s="4">
         <v>736406</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D54" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E54">
         <v>350</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C55" s="22"/>
     </row>
   </sheetData>
@@ -20769,34 +20504,29 @@
   <customProperties>
     <customPr name="DVSECTIONID" r:id="rId1"/>
   </customProperties>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja3" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93:B99"/>
+    <sheetView showRuler="0" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="21" customWidth="1"/>
-    <col min="2" max="2" width="43.83203125" style="22" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" style="22" customWidth="1"/>
     <col min="3" max="3" width="12" style="7" customWidth="1"/>
     <col min="4" max="4" width="17" style="7" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="11.5" style="7"/>
+    <col min="5" max="5" width="18.7109375" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="98">
+    <row r="1" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A1" s="21">
         <v>37622</v>
       </c>
@@ -20804,7 +20534,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
         <v>38245</v>
       </c>
@@ -20812,7 +20542,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>38503</v>
       </c>
@@ -20820,7 +20550,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <v>40515</v>
       </c>
@@ -20828,7 +20558,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <v>40349</v>
       </c>
@@ -20845,7 +20575,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <v>40377</v>
       </c>
@@ -20862,7 +20592,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <v>40379</v>
       </c>
@@ -20873,7 +20603,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <v>40380</v>
       </c>
@@ -20884,7 +20614,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <v>40381</v>
       </c>
@@ -20895,7 +20625,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="28">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <v>40383</v>
       </c>
@@ -20906,7 +20636,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <v>40386</v>
       </c>
@@ -20917,7 +20647,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="13.5" customHeight="1">
+    <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>40387</v>
       </c>
@@ -20928,7 +20658,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="13.5" customHeight="1">
+    <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
         <v>40388</v>
       </c>
@@ -20939,7 +20669,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30.75" customHeight="1">
+    <row r="14" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <v>40569</v>
       </c>
@@ -20947,7 +20677,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="42" customHeight="1">
+    <row r="15" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
         <v>40602</v>
       </c>
@@ -20955,7 +20685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="70">
+    <row r="16" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <v>40646</v>
       </c>
@@ -20963,7 +20693,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28">
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
         <v>40665</v>
       </c>
@@ -20971,7 +20701,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="42">
+    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="21">
         <v>40667</v>
       </c>
@@ -20982,7 +20712,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="21">
         <v>40668</v>
       </c>
@@ -20990,7 +20720,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="21">
         <v>40675</v>
       </c>
@@ -20998,7 +20728,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="21">
         <v>40681</v>
       </c>
@@ -21006,7 +20736,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="21">
         <v>40696</v>
       </c>
@@ -21017,7 +20747,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="21">
         <v>40698</v>
       </c>
@@ -21028,7 +20758,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="21">
         <v>40699</v>
       </c>
@@ -21039,7 +20769,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="21">
         <v>40700</v>
       </c>
@@ -21050,7 +20780,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="21">
         <v>40701</v>
       </c>
@@ -21061,7 +20791,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21">
         <v>40701</v>
       </c>
@@ -21069,7 +20799,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="21">
         <v>40703</v>
       </c>
@@ -21077,7 +20807,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="21">
         <v>40712</v>
       </c>
@@ -21088,7 +20818,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="21">
         <v>40713</v>
       </c>
@@ -21099,7 +20829,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="24">
         <v>40742</v>
       </c>
@@ -21110,7 +20840,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="21">
         <v>40777</v>
       </c>
@@ -21121,7 +20851,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="21">
         <v>40780</v>
       </c>
@@ -21132,7 +20862,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="21">
         <v>40855</v>
       </c>
@@ -21140,7 +20870,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="21">
         <v>40899</v>
       </c>
@@ -21148,7 +20878,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="21">
         <v>40919</v>
       </c>
@@ -21156,7 +20886,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="28">
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="21">
         <v>41035</v>
       </c>
@@ -21167,7 +20897,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="21">
         <v>41050</v>
       </c>
@@ -21175,7 +20905,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="21">
         <v>41107</v>
       </c>
@@ -21183,7 +20913,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="21">
         <v>41135</v>
       </c>
@@ -21191,7 +20921,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="21">
         <v>41150</v>
       </c>
@@ -21199,7 +20929,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="21">
         <v>41154</v>
       </c>
@@ -21207,7 +20937,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="21">
         <v>41157</v>
       </c>
@@ -21215,7 +20945,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="21">
         <v>41167</v>
       </c>
@@ -21229,7 +20959,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="21">
         <v>41167</v>
       </c>
@@ -21243,7 +20973,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="21">
         <v>41171</v>
       </c>
@@ -21251,7 +20981,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="21">
         <v>41192</v>
       </c>
@@ -21259,7 +20989,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="21">
         <v>41197</v>
       </c>
@@ -21270,7 +21000,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="21">
         <v>41206</v>
       </c>
@@ -21278,7 +21008,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="25" customFormat="1">
+    <row r="50" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="24">
         <v>41213</v>
       </c>
@@ -21286,7 +21016,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="25" customFormat="1">
+    <row r="51" spans="1:5" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="24">
         <v>41225</v>
       </c>
@@ -21294,7 +21024,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="25" customFormat="1">
+    <row r="52" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="24">
         <v>41255</v>
       </c>
@@ -21305,7 +21035,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="21">
         <v>41263</v>
       </c>
@@ -21313,7 +21043,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="21">
         <v>41302</v>
       </c>
@@ -21321,7 +21051,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="21">
         <v>41335</v>
       </c>
@@ -21329,7 +21059,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="28">
+    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="21">
         <v>41340</v>
       </c>
@@ -21337,7 +21067,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="21">
         <v>41341</v>
       </c>
@@ -21345,7 +21075,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="21">
         <v>41354</v>
       </c>
@@ -21353,7 +21083,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="21">
         <v>41389</v>
       </c>
@@ -21361,7 +21091,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="21">
         <v>41394</v>
       </c>
@@ -21369,7 +21099,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="28">
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="21">
         <v>41408</v>
       </c>
@@ -21380,7 +21110,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="21">
         <v>41500</v>
       </c>
@@ -21397,7 +21127,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="21">
         <v>41519</v>
       </c>
@@ -21405,7 +21135,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="26">
         <v>41617</v>
       </c>
@@ -21413,7 +21143,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="26">
         <v>41621</v>
       </c>
@@ -21421,7 +21151,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="26">
         <v>41641</v>
       </c>
@@ -21429,7 +21159,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="26">
         <v>41682</v>
       </c>
@@ -21437,7 +21167,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="26">
         <v>41725</v>
       </c>
@@ -21445,7 +21175,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="26">
         <v>41729</v>
       </c>
@@ -21453,7 +21183,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="26">
         <v>41758</v>
       </c>
@@ -21461,7 +21191,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="21">
         <v>41774</v>
       </c>
@@ -21469,7 +21199,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="21">
         <v>41779</v>
       </c>
@@ -21477,7 +21207,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="21">
         <v>41782</v>
       </c>
@@ -21485,7 +21215,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="27">
         <v>41800</v>
       </c>
@@ -21493,7 +21223,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="21">
         <v>41856</v>
       </c>
@@ -21501,7 +21231,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="27">
         <v>41897</v>
       </c>
@@ -21509,7 +21239,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="77" spans="1:2" customFormat="1">
+    <row r="77" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="28">
         <v>41929</v>
       </c>
@@ -21517,7 +21247,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="78" spans="1:2" customFormat="1">
+    <row r="78" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="28">
         <v>41934</v>
       </c>
@@ -21525,7 +21255,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="79" spans="1:2" customFormat="1">
+    <row r="79" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="28">
         <v>41961</v>
       </c>
@@ -21533,7 +21263,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="80" spans="1:2" customFormat="1">
+    <row r="80" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="28">
         <v>41967</v>
       </c>
@@ -21541,7 +21271,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="81" spans="1:5" customFormat="1">
+    <row r="81" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="28">
         <v>41969</v>
       </c>
@@ -21549,7 +21279,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="82" spans="1:5" customFormat="1">
+    <row r="82" spans="1:5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="28">
         <v>41974</v>
       </c>
@@ -21557,7 +21287,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="83" spans="1:5" customFormat="1">
+    <row r="83" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="28">
         <v>41976</v>
       </c>
@@ -21565,7 +21295,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="84" spans="1:5" customFormat="1">
+    <row r="84" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="28">
         <v>41990</v>
       </c>
@@ -21573,7 +21303,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="21">
         <v>42027</v>
       </c>
@@ -21583,7 +21313,7 @@
       <c r="D85"/>
       <c r="E85"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="21">
         <v>42028</v>
       </c>
@@ -21600,7 +21330,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="21">
         <v>42080</v>
       </c>
@@ -21611,7 +21341,7 @@
       <c r="D87"/>
       <c r="E87"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="21">
         <v>42104</v>
       </c>
@@ -21619,7 +21349,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="21">
         <v>42107</v>
       </c>
@@ -21627,7 +21357,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="21">
         <v>42109</v>
       </c>
@@ -21635,7 +21365,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="21">
         <v>42122</v>
       </c>
@@ -21643,26 +21373,26 @@
         <v>203</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="38">
         <v>42161</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="C92" s="4"/>
       <c r="D92"/>
       <c r="E92"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="21">
         <v>42276</v>
       </c>
       <c r="B93" s="22" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="21">
         <v>42388</v>
       </c>
@@ -21670,36 +21400,36 @@
         <v>109</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="21">
         <v>42417</v>
       </c>
       <c r="B95" s="22" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="21">
         <v>42438</v>
       </c>
       <c r="B96" s="22" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="21">
         <v>42439</v>
       </c>
       <c r="B97" s="22" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="21">
         <v>42446</v>
       </c>
       <c r="B98" s="22" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -21709,26 +21439,21 @@
   <customProperties>
     <customPr name="DVSECTIONID" r:id="rId1"/>
   </customProperties>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja4" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:IV9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="BV7" sqref="BV7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:256">
+    <row r="1" spans="1:256" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>IF(icf.157!1:1,"AAAAAF8//gA=",0)</f>
         <v>0</v>
@@ -22754,7 +22479,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="2" spans="1:256">
+    <row r="2" spans="1:256" x14ac:dyDescent="0.25">
       <c r="A2" t="e">
         <f>AND(icf.157!W10,"AAAAAG9/uwA=")</f>
         <v>#VALUE!</v>
@@ -23780,7 +23505,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="3" spans="1:256">
+    <row r="3" spans="1:256" x14ac:dyDescent="0.25">
       <c r="A3" t="e">
         <f>AND(icf.157!S20,"AAAAAHuxawA=")</f>
         <v>#VALUE!</v>
@@ -24806,7 +24531,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="4" spans="1:256">
+    <row r="4" spans="1:256" x14ac:dyDescent="0.25">
       <c r="A4" t="e">
         <f>AND(icf.157!O30,"AAAAAHH/uwA=")</f>
         <v>#VALUE!</v>
@@ -25832,7 +25557,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="1:256">
+    <row r="5" spans="1:256" x14ac:dyDescent="0.25">
       <c r="A5" t="e">
         <f>AND(icf.157!J40,"AAAAAH/s2QA=")</f>
         <v>#VALUE!</v>
@@ -26858,7 +26583,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="1:256">
+    <row r="6" spans="1:256" x14ac:dyDescent="0.25">
       <c r="A6" t="e">
         <f>AND(icf.157!F50,"AAAAAGz/lgA=")</f>
         <v>#VALUE!</v>
@@ -27884,7 +27609,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:256">
+    <row r="7" spans="1:256" x14ac:dyDescent="0.25">
       <c r="A7" t="e">
         <f>AND(Eventos.157!E25,"AAAAAD/WcQA=")</f>
         <v>#VALUE!</v>
@@ -28181,7 +27906,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:256">
+    <row r="8" spans="1:256" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IF(Incidencias.157!20:20,"AAAAAEe//wA=",0)</f>
         <v>AAAAAEe//wA=</v>
@@ -28195,7 +27920,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="9" spans="1:256">
+    <row r="9" spans="1:256" x14ac:dyDescent="0.25">
       <c r="A9" t="e">
         <f>AND(icf.157!#REF!,"AAAAAH88fgA=")</f>
         <v>#REF!</v>
@@ -28419,11 +28144,6 @@
   <customProperties>
     <customPr name="DVSECTIONID" r:id="rId1"/>
   </customProperties>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -28431,21 +28151,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X54"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A32" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="29.1640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="23" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="23" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="5" customFormat="1">
+    <row r="1" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35"/>
       <c r="B1" s="36"/>
       <c r="C1" s="5">
@@ -28515,7 +28235,7 @@
         <v>42109</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -28589,7 +28309,7 @@
         <v>736069</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -28663,7 +28383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -28737,7 +28457,7 @@
         <v>-0.17899999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -28811,7 +28531,7 @@
         <v>-0.33350000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -28885,7 +28605,7 @@
         <v>-0.21299999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -28959,7 +28679,7 @@
         <v>-0.5645</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -29033,7 +28753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -29107,7 +28827,7 @@
         <v>0.33950000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -29181,7 +28901,7 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -29255,7 +28975,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -29329,7 +29049,7 @@
         <v>1580</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -29403,7 +29123,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>12</v>
       </c>
@@ -29477,7 +29197,7 @@
         <v>2.7999999999999999E-8</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -29551,7 +29271,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -29625,7 +29345,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>15</v>
       </c>
@@ -29699,7 +29419,7 @@
         <v>2439</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>16</v>
       </c>
@@ -29773,7 +29493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>17</v>
       </c>
@@ -29847,7 +29567,7 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>18</v>
       </c>
@@ -29921,7 +29641,7 @@
         <v>9320</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>19</v>
       </c>
@@ -29995,7 +29715,7 @@
         <v>13860</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>20</v>
       </c>
@@ -30069,7 +29789,7 @@
         <v>21660</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>21</v>
       </c>
@@ -30143,7 +29863,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="24" spans="1:24">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>22</v>
       </c>
@@ -30217,7 +29937,7 @@
         <v>2972</v>
       </c>
     </row>
-    <row r="25" spans="1:24">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>23</v>
       </c>
@@ -30291,7 +30011,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:24">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>24</v>
       </c>
@@ -30365,7 +30085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:24">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>25</v>
       </c>
@@ -30439,7 +30159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:24">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>26</v>
       </c>
@@ -30513,7 +30233,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="29" spans="1:24">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>27</v>
       </c>
@@ -30587,7 +30307,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="30" spans="1:24">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>28</v>
       </c>
@@ -30661,7 +30381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:24">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>29</v>
       </c>
@@ -30735,7 +30455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:24">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>30</v>
       </c>
@@ -30809,7 +30529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:24">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>31</v>
       </c>
@@ -30883,7 +30603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:24">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>32</v>
       </c>
@@ -30957,7 +30677,7 @@
         <v>7420</v>
       </c>
     </row>
-    <row r="35" spans="1:24">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>33</v>
       </c>
@@ -31031,7 +30751,7 @@
         <v>6025</v>
       </c>
     </row>
-    <row r="36" spans="1:24">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>34</v>
       </c>
@@ -31105,7 +30825,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="37" spans="1:24">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>35</v>
       </c>
@@ -31179,7 +30899,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="1:24">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>36</v>
       </c>
@@ -31253,7 +30973,7 @@
         <v>67397790</v>
       </c>
     </row>
-    <row r="39" spans="1:24">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>37</v>
       </c>
@@ -31327,7 +31047,7 @@
         <v>54644647</v>
       </c>
     </row>
-    <row r="40" spans="1:24">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>38</v>
       </c>
@@ -31401,7 +31121,7 @@
         <v>88722733</v>
       </c>
     </row>
-    <row r="41" spans="1:24">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>39</v>
       </c>
@@ -31475,7 +31195,7 @@
         <v>92846918</v>
       </c>
     </row>
-    <row r="42" spans="1:24">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>40</v>
       </c>
@@ -31549,7 +31269,7 @@
         <v>100533790</v>
       </c>
     </row>
-    <row r="43" spans="1:24">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>41</v>
       </c>
@@ -31623,7 +31343,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="44" spans="1:24">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>42</v>
       </c>
@@ -31697,7 +31417,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="45" spans="1:24">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>43</v>
       </c>
@@ -31771,7 +31491,7 @@
         <v>1732</v>
       </c>
     </row>
-    <row r="46" spans="1:24">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>44</v>
       </c>
@@ -31845,7 +31565,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="47" spans="1:24">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>45</v>
       </c>
@@ -31919,7 +31639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:24">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>46</v>
       </c>
@@ -31993,7 +31713,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:24">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>47</v>
       </c>
@@ -32067,7 +31787,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="50" spans="1:24">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>48</v>
       </c>
@@ -32141,7 +31861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:24">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>49</v>
       </c>
@@ -32215,7 +31935,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:24">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>50</v>
       </c>
@@ -32289,7 +32009,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:24">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>51</v>
       </c>
@@ -32363,7 +32083,7 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="54" spans="1:24">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>52</v>
       </c>
@@ -32437,10 +32157,31 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>15916</v>
+      </c>
+      <c r="B1">
+        <v>16316</v>
+      </c>
+      <c r="C1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New TC and DT change in 2016
</commit_message>
<xml_diff>
--- a/RBCC_E/configs/icf157.xlsx
+++ b/RBCC_E/configs/icf157.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26124"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODE\iberonesia\RBCC_E\configs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aredondas/CODE/iberonesia/RBCC_E/configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="825" yWindow="465" windowWidth="25605" windowHeight="11880" activeTab="6"/>
+    <workbookView xWindow="3200" yWindow="700" windowWidth="25600" windowHeight="11880" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="icf.157" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   <definedNames>
     <definedName name="cfg_s157" localSheetId="5">Cfg_reduced!$C$1:$X$54</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -727,7 +727,7 @@
     <t>Change electric system</t>
   </si>
   <si>
-    <t>Wrong data for lower sza, sighting</t>
+    <t>"Wrong data for lower sza, sighting"</t>
   </si>
 </sst>
 </file>
@@ -735,7 +735,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="172" formatCode="0.00000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -851,7 +851,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -986,9 +986,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1320,21 +1317,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja1"/>
+  <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:BD54"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="AS9" workbookViewId="0">
-      <selection activeCell="BD13" sqref="BD13"/>
+    <sheetView topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="AX26" sqref="AX26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="10"/>
-    <col min="2" max="2" width="29.140625" style="7" customWidth="1"/>
-    <col min="3" max="16384" width="11.28515625" style="13"/>
+    <col min="1" max="1" width="11.3984375" style="10"/>
+    <col min="2" max="2" width="29.19921875" style="7" customWidth="1"/>
+    <col min="3" max="16384" width="11.3984375" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="8">
@@ -1549,7 +1546,7 @@
         <v>42446</v>
       </c>
     </row>
-    <row r="2" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1719,7 +1716,7 @@
         <v>736406</v>
       </c>
     </row>
-    <row r="3" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -1889,7 +1886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -2059,7 +2056,7 @@
         <v>-0.17899999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -2229,7 +2226,7 @@
         <v>-0.33350000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -2399,7 +2396,7 @@
         <v>-0.21299999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -2569,7 +2566,7 @@
         <v>-0.5645</v>
       </c>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -2739,7 +2736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -2909,7 +2906,7 @@
         <v>0.33950000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -3079,7 +3076,7 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -3249,7 +3246,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:56" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:56" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -3419,7 +3416,7 @@
         <v>1590</v>
       </c>
     </row>
-    <row r="13" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -3589,7 +3586,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="1:56" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:56" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>12</v>
       </c>
@@ -3759,7 +3756,7 @@
         <v>2.7999999999999999E-8</v>
       </c>
     </row>
-    <row r="15" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -3929,7 +3926,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="16" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -4099,7 +4096,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>15</v>
       </c>
@@ -4269,7 +4266,7 @@
         <v>2439</v>
       </c>
     </row>
-    <row r="18" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>16</v>
       </c>
@@ -4439,7 +4436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>17</v>
       </c>
@@ -4609,7 +4606,7 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="20" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>18</v>
       </c>
@@ -4779,7 +4776,7 @@
         <v>9320</v>
       </c>
     </row>
-    <row r="21" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>19</v>
       </c>
@@ -4949,7 +4946,7 @@
         <v>13860</v>
       </c>
     </row>
-    <row r="22" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>20</v>
       </c>
@@ -5119,7 +5116,7 @@
         <v>21660</v>
       </c>
     </row>
-    <row r="23" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>21</v>
       </c>
@@ -5289,7 +5286,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="24" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>22</v>
       </c>
@@ -5459,7 +5456,7 @@
         <v>2972</v>
       </c>
     </row>
-    <row r="25" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>23</v>
       </c>
@@ -5629,7 +5626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>24</v>
       </c>
@@ -5799,7 +5796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>25</v>
       </c>
@@ -5969,7 +5966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>26</v>
       </c>
@@ -6139,7 +6136,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>27</v>
       </c>
@@ -6309,7 +6306,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>28</v>
       </c>
@@ -6479,7 +6476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>29</v>
       </c>
@@ -6649,7 +6646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>30</v>
       </c>
@@ -6819,7 +6816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>31</v>
       </c>
@@ -6989,7 +6986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>32</v>
       </c>
@@ -7159,7 +7156,7 @@
         <v>7420</v>
       </c>
     </row>
-    <row r="35" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>33</v>
       </c>
@@ -7329,7 +7326,7 @@
         <v>6025</v>
       </c>
     </row>
-    <row r="36" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>34</v>
       </c>
@@ -7499,7 +7496,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="37" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>35</v>
       </c>
@@ -7669,7 +7666,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>36</v>
       </c>
@@ -7839,7 +7836,7 @@
         <v>67397790</v>
       </c>
     </row>
-    <row r="39" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>37</v>
       </c>
@@ -8009,7 +8006,7 @@
         <v>54644647</v>
       </c>
     </row>
-    <row r="40" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>38</v>
       </c>
@@ -8179,7 +8176,7 @@
         <v>88722733</v>
       </c>
     </row>
-    <row r="41" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>39</v>
       </c>
@@ -8349,7 +8346,7 @@
         <v>92846918</v>
       </c>
     </row>
-    <row r="42" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>40</v>
       </c>
@@ -8519,7 +8516,7 @@
         <v>100533789</v>
       </c>
     </row>
-    <row r="43" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>41</v>
       </c>
@@ -8689,7 +8686,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="44" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>42</v>
       </c>
@@ -8859,7 +8856,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="45" spans="1:56" s="10" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:56" s="10" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>43</v>
       </c>
@@ -9029,7 +9026,7 @@
         <v>1732</v>
       </c>
     </row>
-    <row r="46" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>44</v>
       </c>
@@ -9199,7 +9196,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="47" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>45</v>
       </c>
@@ -9369,7 +9366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>46</v>
       </c>
@@ -9539,7 +9536,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <v>47</v>
       </c>
@@ -9709,7 +9706,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="50" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>48</v>
       </c>
@@ -9879,7 +9876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>49</v>
       </c>
@@ -10049,7 +10046,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>50</v>
       </c>
@@ -10219,7 +10216,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>51</v>
       </c>
@@ -10389,7 +10386,7 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="54" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
         <v>52</v>
       </c>
@@ -10407,7 +10404,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <customProperties>
     <customPr name="DVSECTIONID" r:id="rId1"/>
@@ -10419,18 +10416,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BF54"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="AP14" workbookViewId="0">
-      <selection activeCell="BD29" sqref="BD29"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="AY3" sqref="AY3:AY7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="10"/>
-    <col min="2" max="2" width="29.140625" style="7" customWidth="1"/>
-    <col min="3" max="16384" width="11.28515625" style="13"/>
+    <col min="1" max="1" width="11.3984375" style="10"/>
+    <col min="2" max="2" width="29.19921875" style="7" customWidth="1"/>
+    <col min="3" max="16384" width="11.3984375" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="8">
@@ -10645,7 +10642,7 @@
         <v>42446</v>
       </c>
     </row>
-    <row r="2" spans="1:58" s="10" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:58" s="10" customFormat="1" ht="20" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -10816,7 +10813,7 @@
       </c>
       <c r="BF2" s="39"/>
     </row>
-    <row r="3" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -10986,7 +10983,7 @@
         <v>-1.1000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -11156,7 +11153,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -11326,7 +11323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -11496,7 +11493,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -11666,7 +11663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -11836,7 +11833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -12006,7 +12003,7 @@
         <v>0.33950000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -12176,7 +12173,7 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -12346,7 +12343,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:58" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:58" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -12516,7 +12513,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="13" spans="1:58" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:58" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -12686,7 +12683,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="1:58" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:58" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>12</v>
       </c>
@@ -12835,28 +12832,28 @@
         <v>2.7999999999999999E-8</v>
       </c>
       <c r="AX14" s="17">
-        <v>2.7999999999999999E-8</v>
+        <v>2.6000000000000001E-8</v>
       </c>
       <c r="AY14" s="17">
-        <v>2.7999999999999999E-8</v>
+        <v>2.6000000000000001E-8</v>
       </c>
       <c r="AZ14" s="17">
         <v>2.7999999999999999E-8</v>
       </c>
       <c r="BA14" s="17">
-        <v>2.7999999999999999E-8</v>
+        <v>2.6000000000000001E-8</v>
       </c>
       <c r="BB14" s="17">
-        <v>2.7999999999999999E-8</v>
+        <v>2.6000000000000001E-8</v>
       </c>
       <c r="BC14" s="17">
-        <v>2.7999999999999999E-8</v>
+        <v>2.6000000000000001E-8</v>
       </c>
       <c r="BD14" s="17">
-        <v>2.7999999999999999E-8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:58" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2.6000000000000001E-8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:58" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -13026,7 +13023,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="16" spans="1:58" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:58" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -13196,7 +13193,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>15</v>
       </c>
@@ -13366,7 +13363,7 @@
         <v>2439</v>
       </c>
     </row>
-    <row r="18" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>16</v>
       </c>
@@ -13536,7 +13533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>17</v>
       </c>
@@ -13706,7 +13703,7 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="20" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>18</v>
       </c>
@@ -13876,7 +13873,7 @@
         <v>9320</v>
       </c>
     </row>
-    <row r="21" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>19</v>
       </c>
@@ -14046,7 +14043,7 @@
         <v>13860</v>
       </c>
     </row>
-    <row r="22" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>20</v>
       </c>
@@ -14216,7 +14213,7 @@
         <v>21660</v>
       </c>
     </row>
-    <row r="23" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>21</v>
       </c>
@@ -14386,7 +14383,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="24" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>22</v>
       </c>
@@ -14556,7 +14553,7 @@
         <v>2972</v>
       </c>
     </row>
-    <row r="25" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>23</v>
       </c>
@@ -14726,7 +14723,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>24</v>
       </c>
@@ -14896,7 +14893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>25</v>
       </c>
@@ -15066,7 +15063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>26</v>
       </c>
@@ -15236,7 +15233,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>27</v>
       </c>
@@ -15406,7 +15403,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>28</v>
       </c>
@@ -15576,7 +15573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>29</v>
       </c>
@@ -15746,7 +15743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>30</v>
       </c>
@@ -15916,7 +15913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>31</v>
       </c>
@@ -16086,7 +16083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>32</v>
       </c>
@@ -16256,7 +16253,7 @@
         <v>7420</v>
       </c>
     </row>
-    <row r="35" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>33</v>
       </c>
@@ -16426,7 +16423,7 @@
         <v>6025</v>
       </c>
     </row>
-    <row r="36" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>34</v>
       </c>
@@ -16596,7 +16593,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="37" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>35</v>
       </c>
@@ -16766,7 +16763,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>36</v>
       </c>
@@ -16936,7 +16933,7 @@
         <v>67397790</v>
       </c>
     </row>
-    <row r="39" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>37</v>
       </c>
@@ -17106,7 +17103,7 @@
         <v>54644647</v>
       </c>
     </row>
-    <row r="40" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>38</v>
       </c>
@@ -17276,7 +17273,7 @@
         <v>88722733</v>
       </c>
     </row>
-    <row r="41" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>39</v>
       </c>
@@ -17446,7 +17443,7 @@
         <v>92846918</v>
       </c>
     </row>
-    <row r="42" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>40</v>
       </c>
@@ -17616,7 +17613,7 @@
         <v>100533789</v>
       </c>
     </row>
-    <row r="43" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>41</v>
       </c>
@@ -17786,7 +17783,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="44" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>42</v>
       </c>
@@ -17956,7 +17953,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="45" spans="1:56" s="10" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:56" s="10" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>43</v>
       </c>
@@ -18126,7 +18123,7 @@
         <v>1732</v>
       </c>
     </row>
-    <row r="46" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>44</v>
       </c>
@@ -18296,7 +18293,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="47" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>45</v>
       </c>
@@ -18466,7 +18463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>46</v>
       </c>
@@ -18636,7 +18633,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <v>47</v>
       </c>
@@ -18806,7 +18803,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="50" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>48</v>
       </c>
@@ -18976,7 +18973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>49</v>
       </c>
@@ -19146,7 +19143,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>50</v>
       </c>
@@ -19316,7 +19313,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>51</v>
       </c>
@@ -19486,7 +19483,7 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="54" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
         <v>52</v>
       </c>
@@ -19504,29 +19501,29 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja2"/>
+  <sheetPr codeName="Hoja2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A47" workbookViewId="0">
+    <sheetView topLeftCell="A47" workbookViewId="0">
       <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="11.3984375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" style="4" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5">
         <f t="shared" ref="A1:A32" si="0">+B1-693960</f>
         <v>35431</v>
@@ -19544,7 +19541,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <f t="shared" si="0"/>
         <v>35945</v>
@@ -19562,7 +19559,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <f t="shared" si="0"/>
         <v>36409</v>
@@ -19580,7 +19577,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <f t="shared" si="0"/>
         <v>36682</v>
@@ -19598,7 +19595,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <f t="shared" si="0"/>
         <v>37149</v>
@@ -19616,7 +19613,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <f t="shared" si="0"/>
         <v>37507</v>
@@ -19634,7 +19631,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <f t="shared" si="0"/>
         <v>37877</v>
@@ -19652,7 +19649,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <f t="shared" si="0"/>
         <v>38245</v>
@@ -19670,7 +19667,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <f t="shared" si="0"/>
         <v>38503</v>
@@ -19685,7 +19682,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <f t="shared" si="0"/>
         <v>38615</v>
@@ -19703,7 +19700,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <f t="shared" si="0"/>
         <v>39000</v>
@@ -19721,7 +19718,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <f t="shared" si="0"/>
         <v>39320</v>
@@ -19739,7 +19736,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <f t="shared" si="0"/>
         <v>39981</v>
@@ -19757,7 +19754,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <f t="shared" si="0"/>
         <v>40017</v>
@@ -19775,7 +19772,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <f t="shared" si="0"/>
         <v>40024</v>
@@ -19793,7 +19790,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <f t="shared" si="0"/>
         <v>40060</v>
@@ -19811,7 +19808,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <f t="shared" si="0"/>
         <v>40176</v>
@@ -19829,7 +19826,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <f t="shared" si="0"/>
         <v>40238</v>
@@ -19847,7 +19844,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <f t="shared" si="0"/>
         <v>40267</v>
@@ -19865,7 +19862,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <f t="shared" si="0"/>
         <v>40351</v>
@@ -19883,7 +19880,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <f t="shared" si="0"/>
         <v>40445</v>
@@ -19901,7 +19898,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <f>+B22-693960</f>
         <v>40512</v>
@@ -19919,7 +19916,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <f>+B23-693960</f>
         <v>40571</v>
@@ -19937,7 +19934,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <f t="shared" si="0"/>
         <v>40602</v>
@@ -19955,7 +19952,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <f t="shared" si="0"/>
         <v>40646</v>
@@ -19973,7 +19970,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <f t="shared" si="0"/>
         <v>40681</v>
@@ -19991,7 +19988,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <f t="shared" si="0"/>
         <v>40703</v>
@@ -20009,7 +20006,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <f t="shared" si="0"/>
         <v>40742</v>
@@ -20027,7 +20024,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <f>+B29-693960</f>
         <v>40777</v>
@@ -20045,7 +20042,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <f>+B30-693960</f>
         <v>40780</v>
@@ -20063,7 +20060,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <f t="shared" si="0"/>
         <v>40855</v>
@@ -20081,7 +20078,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <f t="shared" si="0"/>
         <v>40919</v>
@@ -20099,7 +20096,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <f t="shared" ref="A33:A39" si="1">+B33-693960</f>
         <v>41157</v>
@@ -20117,7 +20114,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <f t="shared" si="1"/>
         <v>41206</v>
@@ -20135,7 +20132,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <f t="shared" si="1"/>
         <v>41394</v>
@@ -20153,7 +20150,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <f t="shared" si="1"/>
         <v>41682</v>
@@ -20171,7 +20168,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <f>+B37-693960</f>
         <v>41715</v>
@@ -20189,7 +20186,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <f>+B38-693960</f>
         <v>41758</v>
@@ -20207,7 +20204,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <f t="shared" si="1"/>
         <v>41773</v>
@@ -20225,7 +20222,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
         <v>41782</v>
       </c>
@@ -20242,7 +20239,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="20">
         <f t="shared" ref="A41:A54" si="2">+B41-693960</f>
         <v>41800</v>
@@ -20260,7 +20257,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="20">
         <f t="shared" si="2"/>
         <v>41897</v>
@@ -20278,7 +20275,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="20">
         <f t="shared" si="2"/>
         <v>41991</v>
@@ -20296,7 +20293,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="20">
         <f t="shared" si="2"/>
         <v>42027</v>
@@ -20314,7 +20311,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="20">
         <f t="shared" si="2"/>
         <v>42080</v>
@@ -20332,7 +20329,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="20">
         <f t="shared" si="2"/>
         <v>42104</v>
@@ -20350,7 +20347,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="20">
         <f t="shared" si="2"/>
         <v>42109</v>
@@ -20368,7 +20365,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="20">
         <f t="shared" si="2"/>
         <v>42122</v>
@@ -20386,7 +20383,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="20">
         <f t="shared" si="2"/>
         <v>42161</v>
@@ -20404,7 +20401,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="20">
         <f t="shared" si="2"/>
         <v>42276</v>
@@ -20422,7 +20419,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="20">
         <f t="shared" si="2"/>
         <v>42388</v>
@@ -20440,7 +20437,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="20">
         <f t="shared" si="2"/>
         <v>42417</v>
@@ -20458,7 +20455,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="20">
         <f t="shared" si="2"/>
         <v>42438</v>
@@ -20476,7 +20473,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="20">
         <f t="shared" si="2"/>
         <v>42446</v>
@@ -20494,12 +20491,12 @@
         <v>350</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C55" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <customProperties>
     <customPr name="DVSECTIONID" r:id="rId1"/>
@@ -20509,24 +20506,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja3"/>
+  <sheetPr codeName="Hoja3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="22" customWidth="1"/>
+    <col min="1" max="1" width="11.3984375" style="21" customWidth="1"/>
+    <col min="2" max="2" width="43.796875" style="22" customWidth="1"/>
     <col min="3" max="3" width="12" style="7" customWidth="1"/>
     <col min="4" max="4" width="17" style="7" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="7"/>
+    <col min="5" max="5" width="18.59765625" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="11.3984375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="105" x14ac:dyDescent="0.2">
       <c r="A1" s="21">
         <v>37622</v>
       </c>
@@ -20534,7 +20531,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="21">
         <v>38245</v>
       </c>
@@ -20542,7 +20539,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="21">
         <v>38503</v>
       </c>
@@ -20550,7 +20547,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="21">
         <v>40515</v>
       </c>
@@ -20558,7 +20555,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="21">
         <v>40349</v>
       </c>
@@ -20575,7 +20572,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="21">
         <v>40377</v>
       </c>
@@ -20592,7 +20589,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="21">
         <v>40379</v>
       </c>
@@ -20603,7 +20600,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="21">
         <v>40380</v>
       </c>
@@ -20614,7 +20611,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="21">
         <v>40381</v>
       </c>
@@ -20625,7 +20622,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="21">
         <v>40383</v>
       </c>
@@ -20636,7 +20633,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="21">
         <v>40386</v>
       </c>
@@ -20647,7 +20644,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="21">
         <v>40387</v>
       </c>
@@ -20658,7 +20655,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="21">
         <v>40388</v>
       </c>
@@ -20669,7 +20666,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="21">
         <v>40569</v>
       </c>
@@ -20677,7 +20674,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="21">
         <v>40602</v>
       </c>
@@ -20685,7 +20682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="90" x14ac:dyDescent="0.2">
       <c r="A16" s="21">
         <v>40646</v>
       </c>
@@ -20693,7 +20690,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A17" s="21">
         <v>40665</v>
       </c>
@@ -20701,7 +20698,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A18" s="21">
         <v>40667</v>
       </c>
@@ -20712,7 +20709,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="21">
         <v>40668</v>
       </c>
@@ -20720,7 +20717,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="21">
         <v>40675</v>
       </c>
@@ -20728,7 +20725,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="21">
         <v>40681</v>
       </c>
@@ -20736,7 +20733,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="21">
         <v>40696</v>
       </c>
@@ -20747,7 +20744,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="21">
         <v>40698</v>
       </c>
@@ -20758,7 +20755,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="21">
         <v>40699</v>
       </c>
@@ -20769,7 +20766,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="21">
         <v>40700</v>
       </c>
@@ -20780,7 +20777,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="21">
         <v>40701</v>
       </c>
@@ -20791,7 +20788,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="21">
         <v>40701</v>
       </c>
@@ -20799,7 +20796,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="21">
         <v>40703</v>
       </c>
@@ -20807,7 +20804,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="21">
         <v>40712</v>
       </c>
@@ -20818,7 +20815,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="21">
         <v>40713</v>
       </c>
@@ -20829,7 +20826,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="24">
         <v>40742</v>
       </c>
@@ -20840,7 +20837,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="21">
         <v>40777</v>
       </c>
@@ -20851,7 +20848,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="21">
         <v>40780</v>
       </c>
@@ -20862,7 +20859,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="21">
         <v>40855</v>
       </c>
@@ -20870,7 +20867,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="21">
         <v>40899</v>
       </c>
@@ -20878,7 +20875,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="21">
         <v>40919</v>
       </c>
@@ -20886,7 +20883,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="21">
         <v>41035</v>
       </c>
@@ -20897,7 +20894,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="21">
         <v>41050</v>
       </c>
@@ -20905,7 +20902,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="21">
         <v>41107</v>
       </c>
@@ -20913,7 +20910,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="21">
         <v>41135</v>
       </c>
@@ -20921,7 +20918,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="21">
         <v>41150</v>
       </c>
@@ -20929,7 +20926,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="21">
         <v>41154</v>
       </c>
@@ -20937,7 +20934,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="21">
         <v>41157</v>
       </c>
@@ -20945,7 +20942,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="21">
         <v>41167</v>
       </c>
@@ -20959,7 +20956,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="21">
         <v>41167</v>
       </c>
@@ -20973,7 +20970,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="21">
         <v>41171</v>
       </c>
@@ -20981,7 +20978,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="21">
         <v>41192</v>
       </c>
@@ -20989,7 +20986,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="21">
         <v>41197</v>
       </c>
@@ -21000,7 +20997,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="21">
         <v>41206</v>
       </c>
@@ -21008,7 +21005,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="24">
         <v>41213</v>
       </c>
@@ -21016,7 +21013,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A51" s="24">
         <v>41225</v>
       </c>
@@ -21024,7 +21021,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="24">
         <v>41255</v>
       </c>
@@ -21035,7 +21032,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="21">
         <v>41263</v>
       </c>
@@ -21043,7 +21040,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="21">
         <v>41302</v>
       </c>
@@ -21051,7 +21048,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="21">
         <v>41335</v>
       </c>
@@ -21059,7 +21056,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A56" s="21">
         <v>41340</v>
       </c>
@@ -21067,7 +21064,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="21">
         <v>41341</v>
       </c>
@@ -21075,7 +21072,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A58" s="21">
         <v>41354</v>
       </c>
@@ -21083,7 +21080,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="21">
         <v>41389</v>
       </c>
@@ -21091,7 +21088,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="21">
         <v>41394</v>
       </c>
@@ -21099,7 +21096,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A61" s="21">
         <v>41408</v>
       </c>
@@ -21110,7 +21107,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="21">
         <v>41500</v>
       </c>
@@ -21127,7 +21124,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A63" s="21">
         <v>41519</v>
       </c>
@@ -21135,7 +21132,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="26">
         <v>41617</v>
       </c>
@@ -21143,7 +21140,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="26">
         <v>41621</v>
       </c>
@@ -21151,7 +21148,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="26">
         <v>41641</v>
       </c>
@@ -21159,7 +21156,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A67" s="26">
         <v>41682</v>
       </c>
@@ -21167,7 +21164,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="26">
         <v>41725</v>
       </c>
@@ -21175,7 +21172,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="26">
         <v>41729</v>
       </c>
@@ -21183,7 +21180,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="26">
         <v>41758</v>
       </c>
@@ -21191,7 +21188,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="21">
         <v>41774</v>
       </c>
@@ -21199,7 +21196,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="21">
         <v>41779</v>
       </c>
@@ -21207,7 +21204,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="21">
         <v>41782</v>
       </c>
@@ -21215,7 +21212,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="27">
         <v>41800</v>
       </c>
@@ -21223,7 +21220,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="21">
         <v>41856</v>
       </c>
@@ -21231,7 +21228,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="27">
         <v>41897</v>
       </c>
@@ -21239,7 +21236,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="77" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="28">
         <v>41929</v>
       </c>
@@ -21247,7 +21244,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="78" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="28">
         <v>41934</v>
       </c>
@@ -21255,7 +21252,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="79" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="28">
         <v>41961</v>
       </c>
@@ -21263,7 +21260,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="80" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="28">
         <v>41967</v>
       </c>
@@ -21271,7 +21268,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="81" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="28">
         <v>41969</v>
       </c>
@@ -21279,7 +21276,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="82" spans="1:5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A82" s="28">
         <v>41974</v>
       </c>
@@ -21287,7 +21284,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="83" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="28">
         <v>41976</v>
       </c>
@@ -21295,7 +21292,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="84" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="28">
         <v>41990</v>
       </c>
@@ -21303,7 +21300,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="21">
         <v>42027</v>
       </c>
@@ -21313,7 +21310,7 @@
       <c r="D85"/>
       <c r="E85"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="21">
         <v>42028</v>
       </c>
@@ -21330,7 +21327,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="21">
         <v>42080</v>
       </c>
@@ -21341,7 +21338,7 @@
       <c r="D87"/>
       <c r="E87"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="21">
         <v>42104</v>
       </c>
@@ -21349,7 +21346,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="21">
         <v>42107</v>
       </c>
@@ -21357,7 +21354,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="21">
         <v>42109</v>
       </c>
@@ -21365,7 +21362,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="21">
         <v>42122</v>
       </c>
@@ -21373,7 +21370,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="38">
         <v>42161</v>
       </c>
@@ -21384,7 +21381,7 @@
       <c r="D92"/>
       <c r="E92"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="21">
         <v>42276</v>
       </c>
@@ -21392,7 +21389,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="21">
         <v>42388</v>
       </c>
@@ -21400,7 +21397,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="21">
         <v>42417</v>
       </c>
@@ -21408,7 +21405,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="21">
         <v>42438</v>
       </c>
@@ -21416,7 +21413,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="21">
         <v>42439</v>
       </c>
@@ -21424,7 +21421,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="21">
         <v>42446</v>
       </c>
@@ -21434,7 +21431,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <customProperties>
     <customPr name="DVSECTIONID" r:id="rId1"/>
@@ -21444,16 +21441,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja4"/>
+  <sheetPr codeName="Hoja4" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:IV9"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="BV7" sqref="BV7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:256" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A1">
         <f>IF(icf.157!1:1,"AAAAAF8//gA=",0)</f>
         <v>0</v>
@@ -22479,7 +22476,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="2" spans="1:256" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A2" t="e">
         <f>AND(icf.157!W10,"AAAAAG9/uwA=")</f>
         <v>#VALUE!</v>
@@ -23505,7 +23502,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="3" spans="1:256" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A3" t="e">
         <f>AND(icf.157!S20,"AAAAAHuxawA=")</f>
         <v>#VALUE!</v>
@@ -24531,7 +24528,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="4" spans="1:256" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A4" t="e">
         <f>AND(icf.157!O30,"AAAAAHH/uwA=")</f>
         <v>#VALUE!</v>
@@ -25557,7 +25554,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="1:256" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A5" t="e">
         <f>AND(icf.157!J40,"AAAAAH/s2QA=")</f>
         <v>#VALUE!</v>
@@ -26583,7 +26580,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="1:256" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A6" t="e">
         <f>AND(icf.157!F50,"AAAAAGz/lgA=")</f>
         <v>#VALUE!</v>
@@ -27609,7 +27606,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:256" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A7" t="e">
         <f>AND(Eventos.157!E25,"AAAAAD/WcQA=")</f>
         <v>#VALUE!</v>
@@ -27906,7 +27903,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:256" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>IF(Incidencias.157!20:20,"AAAAAEe//wA=",0)</f>
         <v>AAAAAEe//wA=</v>
@@ -27920,7 +27917,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="9" spans="1:256" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A9" t="e">
         <f>AND(icf.157!#REF!,"AAAAAH88fgA=")</f>
         <v>#REF!</v>
@@ -28140,7 +28137,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
   <customProperties>
     <customPr name="DVSECTIONID" r:id="rId1"/>
   </customProperties>
@@ -28151,21 +28148,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X54"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A32" workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="23" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.796875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="29.19921875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.3984375" customWidth="1"/>
+    <col min="5" max="23" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="35"/>
       <c r="B1" s="36"/>
       <c r="C1" s="5">
@@ -28235,7 +28232,7 @@
         <v>42109</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -28309,7 +28306,7 @@
         <v>736069</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -28383,7 +28380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -28457,7 +28454,7 @@
         <v>-0.17899999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -28531,7 +28528,7 @@
         <v>-0.33350000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -28605,7 +28602,7 @@
         <v>-0.21299999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -28679,7 +28676,7 @@
         <v>-0.5645</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -28753,7 +28750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -28827,7 +28824,7 @@
         <v>0.33950000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -28901,7 +28898,7 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -28975,7 +28972,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -29049,7 +29046,7 @@
         <v>1580</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -29123,7 +29120,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>12</v>
       </c>
@@ -29197,7 +29194,7 @@
         <v>2.7999999999999999E-8</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -29271,7 +29268,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -29345,7 +29342,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>15</v>
       </c>
@@ -29419,7 +29416,7 @@
         <v>2439</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>16</v>
       </c>
@@ -29493,7 +29490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>17</v>
       </c>
@@ -29567,7 +29564,7 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>18</v>
       </c>
@@ -29641,7 +29638,7 @@
         <v>9320</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>19</v>
       </c>
@@ -29715,7 +29712,7 @@
         <v>13860</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>20</v>
       </c>
@@ -29789,7 +29786,7 @@
         <v>21660</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>21</v>
       </c>
@@ -29863,7 +29860,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>22</v>
       </c>
@@ -29937,7 +29934,7 @@
         <v>2972</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>23</v>
       </c>
@@ -30011,7 +30008,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>24</v>
       </c>
@@ -30085,7 +30082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>25</v>
       </c>
@@ -30159,7 +30156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>26</v>
       </c>
@@ -30233,7 +30230,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>27</v>
       </c>
@@ -30307,7 +30304,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>28</v>
       </c>
@@ -30381,7 +30378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>29</v>
       </c>
@@ -30455,7 +30452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>30</v>
       </c>
@@ -30529,7 +30526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>31</v>
       </c>
@@ -30603,7 +30600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>32</v>
       </c>
@@ -30677,7 +30674,7 @@
         <v>7420</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>33</v>
       </c>
@@ -30751,7 +30748,7 @@
         <v>6025</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>34</v>
       </c>
@@ -30825,7 +30822,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>35</v>
       </c>
@@ -30899,7 +30896,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>36</v>
       </c>
@@ -30973,7 +30970,7 @@
         <v>67397790</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>37</v>
       </c>
@@ -31047,7 +31044,7 @@
         <v>54644647</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>38</v>
       </c>
@@ -31121,7 +31118,7 @@
         <v>88722733</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>39</v>
       </c>
@@ -31195,7 +31192,7 @@
         <v>92846918</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>40</v>
       </c>
@@ -31269,7 +31266,7 @@
         <v>100533790</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>41</v>
       </c>
@@ -31343,7 +31340,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>42</v>
       </c>
@@ -31417,7 +31414,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>43</v>
       </c>
@@ -31491,7 +31488,7 @@
         <v>1732</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>44</v>
       </c>
@@ -31565,7 +31562,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>45</v>
       </c>
@@ -31639,7 +31636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>46</v>
       </c>
@@ -31713,7 +31710,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <v>47</v>
       </c>
@@ -31787,7 +31784,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>48</v>
       </c>
@@ -31861,7 +31858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>49</v>
       </c>
@@ -31935,7 +31932,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>50</v>
       </c>
@@ -32009,7 +32006,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>51</v>
       </c>
@@ -32083,7 +32080,7 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
         <v>52</v>
       </c>
@@ -32164,13 +32161,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>15916</v>
       </c>
@@ -32182,6 +32179,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change temperature coeff, dt en alternative
</commit_message>
<xml_diff>
--- a/RBCC_E/configs/icf157.xlsx
+++ b/RBCC_E/configs/icf157.xlsx
@@ -1321,7 +1321,7 @@
   <dimension ref="A1:BD54"/>
   <sheetViews>
     <sheetView topLeftCell="AP1" workbookViewId="0">
-      <selection activeCell="AX26" sqref="AX26"/>
+      <selection activeCell="BD12" sqref="BD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1868,22 +1868,22 @@
         <v>0</v>
       </c>
       <c r="AY3" s="14">
-        <v>0</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="AZ3" s="14">
-        <v>0</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="BA3" s="14">
-        <v>0</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="BB3" s="14">
-        <v>0</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="BC3" s="14">
-        <v>0</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="BD3" s="14">
-        <v>0</v>
+        <v>-1.1000000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.2">
@@ -2038,22 +2038,22 @@
         <v>-0.17899999999999999</v>
       </c>
       <c r="AY4" s="14">
-        <v>-0.17899999999999999</v>
+        <v>-0.6</v>
       </c>
       <c r="AZ4" s="14">
-        <v>-0.17899999999999999</v>
+        <v>-0.6</v>
       </c>
       <c r="BA4" s="14">
-        <v>-0.17899999999999999</v>
+        <v>-0.6</v>
       </c>
       <c r="BB4" s="14">
-        <v>-0.17899999999999999</v>
+        <v>-0.6</v>
       </c>
       <c r="BC4" s="14">
-        <v>-0.17899999999999999</v>
+        <v>-0.6</v>
       </c>
       <c r="BD4" s="14">
-        <v>-0.17899999999999999</v>
+        <v>-0.6</v>
       </c>
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.2">
@@ -2208,22 +2208,22 @@
         <v>-0.33350000000000002</v>
       </c>
       <c r="AY5" s="14">
-        <v>-0.33350000000000002</v>
+        <v>0</v>
       </c>
       <c r="AZ5" s="14">
-        <v>-0.33350000000000002</v>
+        <v>0</v>
       </c>
       <c r="BA5" s="14">
-        <v>-0.33350000000000002</v>
+        <v>0</v>
       </c>
       <c r="BB5" s="14">
-        <v>-0.33350000000000002</v>
+        <v>0</v>
       </c>
       <c r="BC5" s="14">
-        <v>-0.33350000000000002</v>
+        <v>0</v>
       </c>
       <c r="BD5" s="14">
-        <v>-0.33350000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.2">
@@ -2378,22 +2378,22 @@
         <v>-0.21299999999999999</v>
       </c>
       <c r="AY6" s="14">
-        <v>-0.21299999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="AZ6" s="14">
-        <v>-0.21299999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="BA6" s="14">
-        <v>-0.21299999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="BB6" s="14">
-        <v>-0.21299999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="BC6" s="14">
-        <v>-0.21299999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="BD6" s="14">
-        <v>-0.21299999999999999</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.2">
@@ -2548,22 +2548,22 @@
         <v>-0.5645</v>
       </c>
       <c r="AY7" s="14">
-        <v>-0.5645</v>
+        <v>0</v>
       </c>
       <c r="AZ7" s="14">
-        <v>-0.5645</v>
+        <v>0</v>
       </c>
       <c r="BA7" s="14">
-        <v>-0.5645</v>
+        <v>0</v>
       </c>
       <c r="BB7" s="14">
-        <v>-0.5645</v>
+        <v>0</v>
       </c>
       <c r="BC7" s="14">
-        <v>-0.5645</v>
+        <v>0</v>
       </c>
       <c r="BD7" s="14">
-        <v>-0.5645</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:56" x14ac:dyDescent="0.2">
@@ -3398,22 +3398,22 @@
         <v>1580</v>
       </c>
       <c r="AY12" s="7">
-        <v>1590</v>
+        <v>1610</v>
       </c>
       <c r="AZ12" s="7">
-        <v>1590</v>
+        <v>1610</v>
       </c>
       <c r="BA12" s="7">
-        <v>1590</v>
+        <v>1610</v>
       </c>
       <c r="BB12" s="7">
-        <v>1590</v>
+        <v>1610</v>
       </c>
       <c r="BC12" s="7">
-        <v>1590</v>
+        <v>1610</v>
       </c>
       <c r="BD12" s="7">
-        <v>1590</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="13" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -10416,8 +10416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BF54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
-      <selection activeCell="AY3" sqref="AY3:AY7"/>
+    <sheetView tabSelected="1" topLeftCell="AP5" workbookViewId="0">
+      <selection activeCell="BB14" sqref="BB14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12832,19 +12832,19 @@
         <v>2.7999999999999999E-8</v>
       </c>
       <c r="AX14" s="17">
-        <v>2.6000000000000001E-8</v>
+        <v>2.7999999999999999E-8</v>
       </c>
       <c r="AY14" s="17">
-        <v>2.6000000000000001E-8</v>
+        <v>2.7999999999999999E-8</v>
       </c>
       <c r="AZ14" s="17">
         <v>2.7999999999999999E-8</v>
       </c>
       <c r="BA14" s="17">
-        <v>2.6000000000000001E-8</v>
+        <v>2.7999999999999999E-8</v>
       </c>
       <c r="BB14" s="17">
-        <v>2.6000000000000001E-8</v>
+        <v>2.7999999999999999E-8</v>
       </c>
       <c r="BC14" s="17">
         <v>2.6000000000000001E-8</v>
@@ -21659,9 +21659,9 @@
         <f>AND(icf.157!AA2,"AAAAAF8//jM=")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA1">
+      <c r="BA1" t="str">
         <f>IF(icf.157!3:3,"AAAAAF8//jQ=",0)</f>
-        <v>0</v>
+        <v>AAAAAF8//jQ=</v>
       </c>
       <c r="BB1" t="e">
         <f>AND(icf.157!A3,"AAAAAF8//jU=")</f>

</xml_diff>

<commit_message>
updated with winter events
</commit_message>
<xml_diff>
--- a/RBCC_E/configs/icf157.xlsx
+++ b/RBCC_E/configs/icf157.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="700" windowWidth="25600" windowHeight="11880" activeTab="1"/>
+    <workbookView xWindow="3200" yWindow="700" windowWidth="25600" windowHeight="11880" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="icf.157" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="224">
   <si>
     <t>#</t>
   </si>
@@ -729,15 +729,27 @@
   <si>
     <t>"Wrong data for lower sza, sighting"</t>
   </si>
+  <si>
+    <t>"SL Jump"</t>
+  </si>
+  <si>
+    <t>"Bad weather"</t>
+  </si>
+  <si>
+    <t>"157 Roof"</t>
+  </si>
+  <si>
+    <t>"HG replacement"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.00000"/>
+    <numFmt numFmtId="178" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -781,12 +793,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -834,7 +840,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -851,7 +857,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -906,7 +912,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutral" xfId="1" builtinId="28" customBuiltin="1"/>
@@ -1318,20 +1323,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:BD54"/>
+  <dimension ref="A1:BI54"/>
   <sheetViews>
-    <sheetView topLeftCell="AP1" workbookViewId="0">
-      <selection activeCell="BD12" sqref="BD12"/>
+    <sheetView topLeftCell="AT1" workbookViewId="0">
+      <selection activeCell="BI1" sqref="BE1:BI2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.3984375" style="10"/>
-    <col min="2" max="2" width="29.19921875" style="7" customWidth="1"/>
-    <col min="3" max="16384" width="11.3984375" style="13"/>
+    <col min="1" max="1" width="11.5" style="10"/>
+    <col min="2" max="2" width="29.1640625" style="7" customWidth="1"/>
+    <col min="3" max="16384" width="11.5" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:61" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="8">
@@ -1545,8 +1550,23 @@
       <c r="BD1" s="5">
         <v>42446</v>
       </c>
+      <c r="BE1" s="8">
+        <v>42646</v>
+      </c>
+      <c r="BF1" s="8">
+        <v>42661</v>
+      </c>
+      <c r="BG1" s="8">
+        <v>42705</v>
+      </c>
+      <c r="BH1" s="8">
+        <v>42709</v>
+      </c>
+      <c r="BI1" s="8">
+        <v>42710</v>
+      </c>
     </row>
-    <row r="2" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1715,8 +1735,23 @@
       <c r="BD2" s="4">
         <v>736406</v>
       </c>
+      <c r="BE2" s="10">
+        <v>736606</v>
+      </c>
+      <c r="BF2" s="10">
+        <v>736621</v>
+      </c>
+      <c r="BG2" s="10">
+        <v>736665</v>
+      </c>
+      <c r="BH2" s="10">
+        <v>736669</v>
+      </c>
+      <c r="BI2" s="10">
+        <v>736670</v>
+      </c>
     </row>
-    <row r="3" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:61" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -1885,8 +1920,23 @@
       <c r="BD3" s="14">
         <v>-1.1000000000000001</v>
       </c>
+      <c r="BE3" s="14">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="BF3" s="14">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="BG3" s="14">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="BH3" s="14">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="BI3" s="14">
+        <v>-1.1000000000000001</v>
+      </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -2055,8 +2105,23 @@
       <c r="BD4" s="14">
         <v>-0.6</v>
       </c>
+      <c r="BE4" s="14">
+        <v>-0.6</v>
+      </c>
+      <c r="BF4" s="14">
+        <v>-0.6</v>
+      </c>
+      <c r="BG4" s="14">
+        <v>-0.6</v>
+      </c>
+      <c r="BH4" s="14">
+        <v>-0.6</v>
+      </c>
+      <c r="BI4" s="14">
+        <v>-0.6</v>
+      </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -2225,8 +2290,23 @@
       <c r="BD5" s="14">
         <v>0</v>
       </c>
+      <c r="BE5" s="14">
+        <v>0</v>
+      </c>
+      <c r="BF5" s="14">
+        <v>0</v>
+      </c>
+      <c r="BG5" s="14">
+        <v>0</v>
+      </c>
+      <c r="BH5" s="14">
+        <v>0</v>
+      </c>
+      <c r="BI5" s="14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -2395,8 +2475,23 @@
       <c r="BD6" s="14">
         <v>0.3</v>
       </c>
+      <c r="BE6" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="BF6" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="BG6" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="BH6" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="BI6" s="14">
+        <v>0.3</v>
+      </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -2565,8 +2660,23 @@
       <c r="BD7" s="14">
         <v>0</v>
       </c>
+      <c r="BE7" s="14">
+        <v>0</v>
+      </c>
+      <c r="BF7" s="14">
+        <v>0</v>
+      </c>
+      <c r="BG7" s="14">
+        <v>0</v>
+      </c>
+      <c r="BH7" s="14">
+        <v>0</v>
+      </c>
+      <c r="BI7" s="14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -2735,8 +2845,23 @@
       <c r="BD8" s="7">
         <v>0</v>
       </c>
+      <c r="BE8" s="7">
+        <v>0</v>
+      </c>
+      <c r="BF8" s="7">
+        <v>0</v>
+      </c>
+      <c r="BG8" s="7">
+        <v>0</v>
+      </c>
+      <c r="BH8" s="7">
+        <v>0</v>
+      </c>
+      <c r="BI8" s="7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -2905,8 +3030,23 @@
       <c r="BD9" s="7">
         <v>0.33950000000000002</v>
       </c>
+      <c r="BE9" s="7">
+        <v>0.33950000000000002</v>
+      </c>
+      <c r="BF9" s="7">
+        <v>0.33950000000000002</v>
+      </c>
+      <c r="BG9" s="7">
+        <v>0.33950000000000002</v>
+      </c>
+      <c r="BH9" s="7">
+        <v>0.33950000000000002</v>
+      </c>
+      <c r="BI9" s="7">
+        <v>0.33950000000000002</v>
+      </c>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -3075,8 +3215,23 @@
       <c r="BD10" s="7">
         <v>2.35</v>
       </c>
+      <c r="BE10" s="7">
+        <v>2.35</v>
+      </c>
+      <c r="BF10" s="7">
+        <v>2.35</v>
+      </c>
+      <c r="BG10" s="7">
+        <v>2.35</v>
+      </c>
+      <c r="BH10" s="7">
+        <v>2.35</v>
+      </c>
+      <c r="BI10" s="7">
+        <v>2.35</v>
+      </c>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -3245,8 +3400,23 @@
       <c r="BD11" s="7">
         <v>1.1499999999999999</v>
       </c>
+      <c r="BE11" s="7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="BF11" s="7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="BG11" s="7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="BH11" s="7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="BI11" s="7">
+        <v>1.1499999999999999</v>
+      </c>
     </row>
-    <row r="12" spans="1:56" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:61" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -3415,8 +3585,23 @@
       <c r="BD12" s="7">
         <v>1610</v>
       </c>
+      <c r="BE12" s="7">
+        <v>1610</v>
+      </c>
+      <c r="BF12" s="7">
+        <v>1610</v>
+      </c>
+      <c r="BG12" s="7">
+        <v>1610</v>
+      </c>
+      <c r="BH12" s="7">
+        <v>1610</v>
+      </c>
+      <c r="BI12" s="7">
+        <v>1610</v>
+      </c>
     </row>
-    <row r="13" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -3585,8 +3770,23 @@
       <c r="BD13" s="7">
         <v>225</v>
       </c>
+      <c r="BE13" s="7">
+        <v>225</v>
+      </c>
+      <c r="BF13" s="7">
+        <v>225</v>
+      </c>
+      <c r="BG13" s="7">
+        <v>225</v>
+      </c>
+      <c r="BH13" s="7">
+        <v>225</v>
+      </c>
+      <c r="BI13" s="7">
+        <v>225</v>
+      </c>
     </row>
-    <row r="14" spans="1:56" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:61" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>12</v>
       </c>
@@ -3755,8 +3955,23 @@
       <c r="BD14" s="17">
         <v>2.7999999999999999E-8</v>
       </c>
+      <c r="BE14" s="17">
+        <v>2.7999999999999999E-8</v>
+      </c>
+      <c r="BF14" s="17">
+        <v>2.7999999999999999E-8</v>
+      </c>
+      <c r="BG14" s="17">
+        <v>2.7999999999999999E-8</v>
+      </c>
+      <c r="BH14" s="17">
+        <v>2.7999999999999999E-8</v>
+      </c>
+      <c r="BI14" s="17">
+        <v>2.7999999999999999E-8</v>
+      </c>
     </row>
-    <row r="15" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:61" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -3925,8 +4140,23 @@
       <c r="BD15" s="7">
         <v>1026</v>
       </c>
+      <c r="BE15" s="7">
+        <v>1026</v>
+      </c>
+      <c r="BF15" s="7">
+        <v>1026</v>
+      </c>
+      <c r="BG15" s="7">
+        <v>1026</v>
+      </c>
+      <c r="BH15" s="7">
+        <v>1026</v>
+      </c>
+      <c r="BI15" s="7">
+        <v>1026</v>
+      </c>
     </row>
-    <row r="16" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:61" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -4095,8 +4325,23 @@
       <c r="BD16" s="7">
         <v>96</v>
       </c>
+      <c r="BE16" s="7">
+        <v>96</v>
+      </c>
+      <c r="BF16" s="7">
+        <v>96</v>
+      </c>
+      <c r="BG16" s="7">
+        <v>96</v>
+      </c>
+      <c r="BH16" s="7">
+        <v>96</v>
+      </c>
+      <c r="BI16" s="7">
+        <v>96</v>
+      </c>
     </row>
-    <row r="17" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:61" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>15</v>
       </c>
@@ -4265,8 +4510,23 @@
       <c r="BD17" s="7">
         <v>2439</v>
       </c>
+      <c r="BE17" s="7">
+        <v>2439</v>
+      </c>
+      <c r="BF17" s="7">
+        <v>2439</v>
+      </c>
+      <c r="BG17" s="7">
+        <v>2439</v>
+      </c>
+      <c r="BH17" s="7">
+        <v>2439</v>
+      </c>
+      <c r="BI17" s="7">
+        <v>2439</v>
+      </c>
     </row>
-    <row r="18" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:61" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>16</v>
       </c>
@@ -4435,8 +4695,23 @@
       <c r="BD18" s="7">
         <v>0</v>
       </c>
+      <c r="BE18" s="7">
+        <v>0</v>
+      </c>
+      <c r="BF18" s="7">
+        <v>0</v>
+      </c>
+      <c r="BG18" s="7">
+        <v>0</v>
+      </c>
+      <c r="BH18" s="7">
+        <v>0</v>
+      </c>
+      <c r="BI18" s="7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:61" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>17</v>
       </c>
@@ -4605,8 +4880,23 @@
       <c r="BD19" s="10">
         <v>4300</v>
       </c>
+      <c r="BE19" s="10">
+        <v>4300</v>
+      </c>
+      <c r="BF19" s="10">
+        <v>4300</v>
+      </c>
+      <c r="BG19" s="10">
+        <v>4300</v>
+      </c>
+      <c r="BH19" s="10">
+        <v>4300</v>
+      </c>
+      <c r="BI19" s="10">
+        <v>4300</v>
+      </c>
     </row>
-    <row r="20" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:61" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>18</v>
       </c>
@@ -4775,8 +5065,23 @@
       <c r="BD20" s="10">
         <v>9320</v>
       </c>
+      <c r="BE20" s="10">
+        <v>9320</v>
+      </c>
+      <c r="BF20" s="10">
+        <v>9320</v>
+      </c>
+      <c r="BG20" s="10">
+        <v>9320</v>
+      </c>
+      <c r="BH20" s="10">
+        <v>9320</v>
+      </c>
+      <c r="BI20" s="10">
+        <v>9320</v>
+      </c>
     </row>
-    <row r="21" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:61" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>19</v>
       </c>
@@ -4945,8 +5250,23 @@
       <c r="BD21" s="10">
         <v>13860</v>
       </c>
+      <c r="BE21" s="10">
+        <v>13860</v>
+      </c>
+      <c r="BF21" s="10">
+        <v>13860</v>
+      </c>
+      <c r="BG21" s="10">
+        <v>13860</v>
+      </c>
+      <c r="BH21" s="10">
+        <v>13860</v>
+      </c>
+      <c r="BI21" s="10">
+        <v>13860</v>
+      </c>
     </row>
-    <row r="22" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:61" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>20</v>
       </c>
@@ -5115,8 +5435,23 @@
       <c r="BD22" s="10">
         <v>21660</v>
       </c>
+      <c r="BE22" s="10">
+        <v>21660</v>
+      </c>
+      <c r="BF22" s="10">
+        <v>21660</v>
+      </c>
+      <c r="BG22" s="10">
+        <v>21660</v>
+      </c>
+      <c r="BH22" s="10">
+        <v>21660</v>
+      </c>
+      <c r="BI22" s="10">
+        <v>21660</v>
+      </c>
     </row>
-    <row r="23" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:61" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>21</v>
       </c>
@@ -5285,8 +5620,23 @@
       <c r="BD23" s="10">
         <v>25000</v>
       </c>
+      <c r="BE23" s="10">
+        <v>25000</v>
+      </c>
+      <c r="BF23" s="10">
+        <v>25000</v>
+      </c>
+      <c r="BG23" s="10">
+        <v>25000</v>
+      </c>
+      <c r="BH23" s="10">
+        <v>25000</v>
+      </c>
+      <c r="BI23" s="10">
+        <v>25000</v>
+      </c>
     </row>
-    <row r="24" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>22</v>
       </c>
@@ -5455,8 +5805,23 @@
       <c r="BD24" s="7">
         <v>2972</v>
       </c>
+      <c r="BE24" s="7">
+        <v>2972</v>
+      </c>
+      <c r="BF24" s="7">
+        <v>2972</v>
+      </c>
+      <c r="BG24" s="7">
+        <v>2972</v>
+      </c>
+      <c r="BH24" s="7">
+        <v>2972</v>
+      </c>
+      <c r="BI24" s="7">
+        <v>2972</v>
+      </c>
     </row>
-    <row r="25" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>23</v>
       </c>
@@ -5625,8 +5990,23 @@
       <c r="BD25" s="7">
         <v>3</v>
       </c>
+      <c r="BE25" s="7">
+        <v>3</v>
+      </c>
+      <c r="BF25" s="7">
+        <v>3</v>
+      </c>
+      <c r="BG25" s="7">
+        <v>3</v>
+      </c>
+      <c r="BH25" s="7">
+        <v>3</v>
+      </c>
+      <c r="BI25" s="7">
+        <v>3</v>
+      </c>
     </row>
-    <row r="26" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>24</v>
       </c>
@@ -5795,8 +6175,23 @@
       <c r="BD26" s="7">
         <v>0</v>
       </c>
+      <c r="BE26" s="7">
+        <v>0</v>
+      </c>
+      <c r="BF26" s="7">
+        <v>0</v>
+      </c>
+      <c r="BG26" s="7">
+        <v>0</v>
+      </c>
+      <c r="BH26" s="7">
+        <v>0</v>
+      </c>
+      <c r="BI26" s="7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>25</v>
       </c>
@@ -5965,8 +6360,23 @@
       <c r="BD27" s="14">
         <v>0</v>
       </c>
+      <c r="BE27" s="14">
+        <v>0</v>
+      </c>
+      <c r="BF27" s="14">
+        <v>0</v>
+      </c>
+      <c r="BG27" s="14">
+        <v>0</v>
+      </c>
+      <c r="BH27" s="14">
+        <v>0</v>
+      </c>
+      <c r="BI27" s="14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>26</v>
       </c>
@@ -6135,8 +6545,23 @@
       <c r="BD28" s="7">
         <v>342</v>
       </c>
+      <c r="BE28" s="7">
+        <v>342</v>
+      </c>
+      <c r="BF28" s="7">
+        <v>342</v>
+      </c>
+      <c r="BG28" s="7">
+        <v>342</v>
+      </c>
+      <c r="BH28" s="7">
+        <v>342</v>
+      </c>
+      <c r="BI28" s="7">
+        <v>342</v>
+      </c>
     </row>
-    <row r="29" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>27</v>
       </c>
@@ -6305,8 +6730,23 @@
       <c r="BD29" s="14">
         <v>580</v>
       </c>
+      <c r="BE29" s="14">
+        <v>580</v>
+      </c>
+      <c r="BF29" s="14">
+        <v>580</v>
+      </c>
+      <c r="BG29" s="14">
+        <v>580</v>
+      </c>
+      <c r="BH29" s="14">
+        <v>580</v>
+      </c>
+      <c r="BI29" s="14">
+        <v>580</v>
+      </c>
     </row>
-    <row r="30" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>28</v>
       </c>
@@ -6475,8 +6915,23 @@
       <c r="BD30" s="14">
         <v>0</v>
       </c>
+      <c r="BE30" s="14">
+        <v>0</v>
+      </c>
+      <c r="BF30" s="14">
+        <v>0</v>
+      </c>
+      <c r="BG30" s="14">
+        <v>0</v>
+      </c>
+      <c r="BH30" s="14">
+        <v>0</v>
+      </c>
+      <c r="BI30" s="14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>29</v>
       </c>
@@ -6645,8 +7100,23 @@
       <c r="BD31" s="14">
         <v>0</v>
       </c>
+      <c r="BE31" s="14">
+        <v>0</v>
+      </c>
+      <c r="BF31" s="14">
+        <v>0</v>
+      </c>
+      <c r="BG31" s="14">
+        <v>0</v>
+      </c>
+      <c r="BH31" s="14">
+        <v>0</v>
+      </c>
+      <c r="BI31" s="14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>30</v>
       </c>
@@ -6815,8 +7285,23 @@
       <c r="BD32" s="14">
         <v>0</v>
       </c>
+      <c r="BE32" s="14">
+        <v>0</v>
+      </c>
+      <c r="BF32" s="14">
+        <v>0</v>
+      </c>
+      <c r="BG32" s="14">
+        <v>0</v>
+      </c>
+      <c r="BH32" s="14">
+        <v>0</v>
+      </c>
+      <c r="BI32" s="14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>31</v>
       </c>
@@ -6985,8 +7470,23 @@
       <c r="BD33" s="14">
         <v>0</v>
       </c>
+      <c r="BE33" s="14">
+        <v>0</v>
+      </c>
+      <c r="BF33" s="14">
+        <v>0</v>
+      </c>
+      <c r="BG33" s="14">
+        <v>0</v>
+      </c>
+      <c r="BH33" s="14">
+        <v>0</v>
+      </c>
+      <c r="BI33" s="14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>32</v>
       </c>
@@ -7155,8 +7655,23 @@
       <c r="BD34" s="14">
         <v>7420</v>
       </c>
+      <c r="BE34" s="14">
+        <v>7420</v>
+      </c>
+      <c r="BF34" s="14">
+        <v>7420</v>
+      </c>
+      <c r="BG34" s="14">
+        <v>7420</v>
+      </c>
+      <c r="BH34" s="14">
+        <v>7420</v>
+      </c>
+      <c r="BI34" s="14">
+        <v>7420</v>
+      </c>
     </row>
-    <row r="35" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>33</v>
       </c>
@@ -7325,8 +7840,23 @@
       <c r="BD35" s="7">
         <v>6025</v>
       </c>
+      <c r="BE35" s="7">
+        <v>6025</v>
+      </c>
+      <c r="BF35" s="7">
+        <v>6025</v>
+      </c>
+      <c r="BG35" s="7">
+        <v>6025</v>
+      </c>
+      <c r="BH35" s="7">
+        <v>6025</v>
+      </c>
+      <c r="BI35" s="7">
+        <v>6025</v>
+      </c>
     </row>
-    <row r="36" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>34</v>
       </c>
@@ -7495,8 +8025,23 @@
       <c r="BD36" s="7">
         <v>178</v>
       </c>
+      <c r="BE36" s="7">
+        <v>178</v>
+      </c>
+      <c r="BF36" s="7">
+        <v>178</v>
+      </c>
+      <c r="BG36" s="7">
+        <v>178</v>
+      </c>
+      <c r="BH36" s="7">
+        <v>178</v>
+      </c>
+      <c r="BI36" s="7">
+        <v>178</v>
+      </c>
     </row>
-    <row r="37" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>35</v>
       </c>
@@ -7665,8 +8210,23 @@
       <c r="BD37" s="7" t="s">
         <v>193</v>
       </c>
+      <c r="BE37" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BF37" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BG37" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BH37" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BI37" s="7" t="s">
+        <v>193</v>
+      </c>
     </row>
-    <row r="38" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>36</v>
       </c>
@@ -7835,8 +8395,23 @@
       <c r="BD38" s="7">
         <v>67397790</v>
       </c>
+      <c r="BE38" s="7">
+        <v>67397790</v>
+      </c>
+      <c r="BF38" s="7">
+        <v>67397790</v>
+      </c>
+      <c r="BG38" s="7">
+        <v>67397790</v>
+      </c>
+      <c r="BH38" s="7">
+        <v>67397790</v>
+      </c>
+      <c r="BI38" s="7">
+        <v>67397790</v>
+      </c>
     </row>
-    <row r="39" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>37</v>
       </c>
@@ -8005,8 +8580,23 @@
       <c r="BD39" s="7">
         <v>54644647</v>
       </c>
+      <c r="BE39" s="7">
+        <v>54644647</v>
+      </c>
+      <c r="BF39" s="7">
+        <v>54644647</v>
+      </c>
+      <c r="BG39" s="7">
+        <v>54644647</v>
+      </c>
+      <c r="BH39" s="7">
+        <v>54644647</v>
+      </c>
+      <c r="BI39" s="7">
+        <v>54644647</v>
+      </c>
     </row>
-    <row r="40" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>38</v>
       </c>
@@ -8175,8 +8765,23 @@
       <c r="BD40" s="7">
         <v>88722733</v>
       </c>
+      <c r="BE40" s="7">
+        <v>88722733</v>
+      </c>
+      <c r="BF40" s="7">
+        <v>88722733</v>
+      </c>
+      <c r="BG40" s="7">
+        <v>88722733</v>
+      </c>
+      <c r="BH40" s="7">
+        <v>88722733</v>
+      </c>
+      <c r="BI40" s="7">
+        <v>88722733</v>
+      </c>
     </row>
-    <row r="41" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>39</v>
       </c>
@@ -8345,8 +8950,23 @@
       <c r="BD41" s="7">
         <v>92846918</v>
       </c>
+      <c r="BE41" s="7">
+        <v>92846918</v>
+      </c>
+      <c r="BF41" s="7">
+        <v>92846918</v>
+      </c>
+      <c r="BG41" s="7">
+        <v>92846918</v>
+      </c>
+      <c r="BH41" s="7">
+        <v>92846918</v>
+      </c>
+      <c r="BI41" s="7">
+        <v>92846918</v>
+      </c>
     </row>
-    <row r="42" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>40</v>
       </c>
@@ -8515,8 +9135,23 @@
       <c r="BD42" s="7">
         <v>100533789</v>
       </c>
+      <c r="BE42" s="7">
+        <v>100533789</v>
+      </c>
+      <c r="BF42" s="7">
+        <v>100533789</v>
+      </c>
+      <c r="BG42" s="7">
+        <v>100533789</v>
+      </c>
+      <c r="BH42" s="7">
+        <v>100533789</v>
+      </c>
+      <c r="BI42" s="7">
+        <v>100533789</v>
+      </c>
     </row>
-    <row r="43" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>41</v>
       </c>
@@ -8685,8 +9320,23 @@
       <c r="BD43" s="14">
         <v>0.998</v>
       </c>
+      <c r="BE43" s="14">
+        <v>0.998</v>
+      </c>
+      <c r="BF43" s="14">
+        <v>0.998</v>
+      </c>
+      <c r="BG43" s="14">
+        <v>0.998</v>
+      </c>
+      <c r="BH43" s="14">
+        <v>0.998</v>
+      </c>
+      <c r="BI43" s="14">
+        <v>0.998</v>
+      </c>
     </row>
-    <row r="44" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>42</v>
       </c>
@@ -8855,8 +9505,23 @@
       <c r="BD44" s="14">
         <v>-10</v>
       </c>
+      <c r="BE44" s="14">
+        <v>-10</v>
+      </c>
+      <c r="BF44" s="14">
+        <v>-10</v>
+      </c>
+      <c r="BG44" s="14">
+        <v>-10</v>
+      </c>
+      <c r="BH44" s="14">
+        <v>-10</v>
+      </c>
+      <c r="BI44" s="14">
+        <v>-10</v>
+      </c>
     </row>
-    <row r="45" spans="1:56" s="10" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:61" s="10" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>43</v>
       </c>
@@ -9025,8 +9690,23 @@
       <c r="BD45" s="7">
         <v>1732</v>
       </c>
+      <c r="BE45" s="7">
+        <v>1732</v>
+      </c>
+      <c r="BF45" s="7">
+        <v>1732</v>
+      </c>
+      <c r="BG45" s="7">
+        <v>1732</v>
+      </c>
+      <c r="BH45" s="7">
+        <v>1732</v>
+      </c>
+      <c r="BI45" s="7">
+        <v>1732</v>
+      </c>
     </row>
-    <row r="46" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>44</v>
       </c>
@@ -9195,8 +9875,23 @@
       <c r="BD46" s="7">
         <v>250</v>
       </c>
+      <c r="BE46" s="7">
+        <v>250</v>
+      </c>
+      <c r="BF46" s="7">
+        <v>250</v>
+      </c>
+      <c r="BG46" s="7">
+        <v>250</v>
+      </c>
+      <c r="BH46" s="7">
+        <v>250</v>
+      </c>
+      <c r="BI46" s="7">
+        <v>250</v>
+      </c>
     </row>
-    <row r="47" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>45</v>
       </c>
@@ -9365,8 +10060,23 @@
       <c r="BD47" s="7">
         <v>0</v>
       </c>
+      <c r="BE47" s="7">
+        <v>0</v>
+      </c>
+      <c r="BF47" s="7">
+        <v>0</v>
+      </c>
+      <c r="BG47" s="7">
+        <v>0</v>
+      </c>
+      <c r="BH47" s="7">
+        <v>0</v>
+      </c>
+      <c r="BI47" s="7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>46</v>
       </c>
@@ -9535,8 +10245,23 @@
       <c r="BD48" s="7">
         <v>64</v>
       </c>
+      <c r="BE48" s="7">
+        <v>64</v>
+      </c>
+      <c r="BF48" s="7">
+        <v>64</v>
+      </c>
+      <c r="BG48" s="7">
+        <v>64</v>
+      </c>
+      <c r="BH48" s="7">
+        <v>64</v>
+      </c>
+      <c r="BI48" s="7">
+        <v>64</v>
+      </c>
     </row>
-    <row r="49" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <v>47</v>
       </c>
@@ -9705,8 +10430,23 @@
       <c r="BD49" s="7">
         <v>256</v>
       </c>
+      <c r="BE49" s="7">
+        <v>256</v>
+      </c>
+      <c r="BF49" s="7">
+        <v>256</v>
+      </c>
+      <c r="BG49" s="7">
+        <v>256</v>
+      </c>
+      <c r="BH49" s="7">
+        <v>256</v>
+      </c>
+      <c r="BI49" s="7">
+        <v>256</v>
+      </c>
     </row>
-    <row r="50" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>48</v>
       </c>
@@ -9875,8 +10615,23 @@
       <c r="BD50" s="7">
         <v>0</v>
       </c>
+      <c r="BE50" s="7">
+        <v>0</v>
+      </c>
+      <c r="BF50" s="7">
+        <v>0</v>
+      </c>
+      <c r="BG50" s="7">
+        <v>0</v>
+      </c>
+      <c r="BH50" s="7">
+        <v>0</v>
+      </c>
+      <c r="BI50" s="7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="51" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>49</v>
       </c>
@@ -10045,8 +10800,23 @@
       <c r="BD51" s="7">
         <v>64</v>
       </c>
+      <c r="BE51" s="7">
+        <v>64</v>
+      </c>
+      <c r="BF51" s="7">
+        <v>64</v>
+      </c>
+      <c r="BG51" s="7">
+        <v>64</v>
+      </c>
+      <c r="BH51" s="7">
+        <v>64</v>
+      </c>
+      <c r="BI51" s="7">
+        <v>64</v>
+      </c>
     </row>
-    <row r="52" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>50</v>
       </c>
@@ -10215,8 +10985,23 @@
       <c r="BD52" s="7">
         <v>56</v>
       </c>
+      <c r="BE52" s="7">
+        <v>56</v>
+      </c>
+      <c r="BF52" s="7">
+        <v>56</v>
+      </c>
+      <c r="BG52" s="7">
+        <v>56</v>
+      </c>
+      <c r="BH52" s="7">
+        <v>56</v>
+      </c>
+      <c r="BI52" s="7">
+        <v>56</v>
+      </c>
     </row>
-    <row r="53" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>51</v>
       </c>
@@ -10385,8 +11170,23 @@
       <c r="BD53" s="7">
         <v>2226</v>
       </c>
+      <c r="BE53" s="7">
+        <v>2226</v>
+      </c>
+      <c r="BF53" s="7">
+        <v>2226</v>
+      </c>
+      <c r="BG53" s="7">
+        <v>2226</v>
+      </c>
+      <c r="BH53" s="7">
+        <v>2226</v>
+      </c>
+      <c r="BI53" s="7">
+        <v>2226</v>
+      </c>
     </row>
-    <row r="54" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
         <v>52</v>
       </c>
@@ -10414,20 +11214,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF54"/>
+  <dimension ref="A1:BI54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP5" workbookViewId="0">
-      <selection activeCell="BB14" sqref="BB14"/>
+    <sheetView topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="BI3" sqref="BI3:BI53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.3984375" style="10"/>
-    <col min="2" max="2" width="29.19921875" style="7" customWidth="1"/>
-    <col min="3" max="16384" width="11.3984375" style="13"/>
+    <col min="1" max="1" width="11.5" style="10"/>
+    <col min="2" max="2" width="29.1640625" style="7" customWidth="1"/>
+    <col min="3" max="16384" width="11.5" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:61" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="8">
@@ -10641,8 +11441,23 @@
       <c r="BD1" s="5">
         <v>42446</v>
       </c>
+      <c r="BE1" s="8">
+        <v>42646</v>
+      </c>
+      <c r="BF1" s="8">
+        <v>42661</v>
+      </c>
+      <c r="BG1" s="8">
+        <v>42705</v>
+      </c>
+      <c r="BH1" s="8">
+        <v>42709</v>
+      </c>
+      <c r="BI1" s="8">
+        <v>42710</v>
+      </c>
     </row>
-    <row r="2" spans="1:58" s="10" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -10811,9 +11626,23 @@
       <c r="BD2" s="4">
         <v>736406</v>
       </c>
-      <c r="BF2" s="39"/>
+      <c r="BE2" s="10">
+        <v>736606</v>
+      </c>
+      <c r="BF2" s="10">
+        <v>736621</v>
+      </c>
+      <c r="BG2" s="10">
+        <v>736665</v>
+      </c>
+      <c r="BH2" s="10">
+        <v>736669</v>
+      </c>
+      <c r="BI2" s="10">
+        <v>736670</v>
+      </c>
     </row>
-    <row r="3" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:61" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -10982,8 +11811,23 @@
       <c r="BD3" s="14">
         <v>-1.1000000000000001</v>
       </c>
+      <c r="BE3" s="14">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="BF3" s="14">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="BG3" s="14">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="BH3" s="14">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="BI3" s="14">
+        <v>-1.1000000000000001</v>
+      </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -11152,8 +11996,23 @@
       <c r="BD4" s="14">
         <v>-0.6</v>
       </c>
+      <c r="BE4" s="14">
+        <v>-0.6</v>
+      </c>
+      <c r="BF4" s="14">
+        <v>-0.6</v>
+      </c>
+      <c r="BG4" s="14">
+        <v>-0.6</v>
+      </c>
+      <c r="BH4" s="14">
+        <v>-0.6</v>
+      </c>
+      <c r="BI4" s="14">
+        <v>-0.6</v>
+      </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -11322,8 +12181,23 @@
       <c r="BD5" s="14">
         <v>0</v>
       </c>
+      <c r="BE5" s="14">
+        <v>0</v>
+      </c>
+      <c r="BF5" s="14">
+        <v>0</v>
+      </c>
+      <c r="BG5" s="14">
+        <v>0</v>
+      </c>
+      <c r="BH5" s="14">
+        <v>0</v>
+      </c>
+      <c r="BI5" s="14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -11492,8 +12366,23 @@
       <c r="BD6" s="14">
         <v>0.3</v>
       </c>
+      <c r="BE6" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="BF6" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="BG6" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="BH6" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="BI6" s="14">
+        <v>0.3</v>
+      </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -11662,8 +12551,23 @@
       <c r="BD7" s="14">
         <v>0</v>
       </c>
+      <c r="BE7" s="14">
+        <v>0</v>
+      </c>
+      <c r="BF7" s="14">
+        <v>0</v>
+      </c>
+      <c r="BG7" s="14">
+        <v>0</v>
+      </c>
+      <c r="BH7" s="14">
+        <v>0</v>
+      </c>
+      <c r="BI7" s="14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -11832,8 +12736,23 @@
       <c r="BD8" s="7">
         <v>0</v>
       </c>
+      <c r="BE8" s="7">
+        <v>0</v>
+      </c>
+      <c r="BF8" s="7">
+        <v>0</v>
+      </c>
+      <c r="BG8" s="7">
+        <v>0</v>
+      </c>
+      <c r="BH8" s="7">
+        <v>0</v>
+      </c>
+      <c r="BI8" s="7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -12002,8 +12921,23 @@
       <c r="BD9" s="7">
         <v>0.33950000000000002</v>
       </c>
+      <c r="BE9" s="7">
+        <v>0.33950000000000002</v>
+      </c>
+      <c r="BF9" s="7">
+        <v>0.33950000000000002</v>
+      </c>
+      <c r="BG9" s="7">
+        <v>0.33950000000000002</v>
+      </c>
+      <c r="BH9" s="7">
+        <v>0.33950000000000002</v>
+      </c>
+      <c r="BI9" s="7">
+        <v>0.33950000000000002</v>
+      </c>
     </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -12172,8 +13106,23 @@
       <c r="BD10" s="7">
         <v>2.35</v>
       </c>
+      <c r="BE10" s="7">
+        <v>2.35</v>
+      </c>
+      <c r="BF10" s="7">
+        <v>2.35</v>
+      </c>
+      <c r="BG10" s="7">
+        <v>2.35</v>
+      </c>
+      <c r="BH10" s="7">
+        <v>2.35</v>
+      </c>
+      <c r="BI10" s="7">
+        <v>2.35</v>
+      </c>
     </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -12342,8 +13291,23 @@
       <c r="BD11" s="7">
         <v>1.1499999999999999</v>
       </c>
+      <c r="BE11" s="7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="BF11" s="7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="BG11" s="7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="BH11" s="7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="BI11" s="7">
+        <v>1.1499999999999999</v>
+      </c>
     </row>
-    <row r="12" spans="1:58" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:61" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -12512,8 +13476,23 @@
       <c r="BD12" s="7">
         <v>1610</v>
       </c>
+      <c r="BE12" s="7">
+        <v>1610</v>
+      </c>
+      <c r="BF12" s="7">
+        <v>1610</v>
+      </c>
+      <c r="BG12" s="7">
+        <v>1610</v>
+      </c>
+      <c r="BH12" s="7">
+        <v>1610</v>
+      </c>
+      <c r="BI12" s="7">
+        <v>1610</v>
+      </c>
     </row>
-    <row r="13" spans="1:58" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -12682,8 +13661,23 @@
       <c r="BD13" s="7">
         <v>225</v>
       </c>
+      <c r="BE13" s="7">
+        <v>225</v>
+      </c>
+      <c r="BF13" s="7">
+        <v>225</v>
+      </c>
+      <c r="BG13" s="7">
+        <v>225</v>
+      </c>
+      <c r="BH13" s="7">
+        <v>225</v>
+      </c>
+      <c r="BI13" s="7">
+        <v>225</v>
+      </c>
     </row>
-    <row r="14" spans="1:58" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:61" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>12</v>
       </c>
@@ -12852,8 +13846,23 @@
       <c r="BD14" s="17">
         <v>2.6000000000000001E-8</v>
       </c>
+      <c r="BE14" s="17">
+        <v>2.6000000000000001E-8</v>
+      </c>
+      <c r="BF14" s="17">
+        <v>2.6000000000000001E-8</v>
+      </c>
+      <c r="BG14" s="17">
+        <v>2.6000000000000001E-8</v>
+      </c>
+      <c r="BH14" s="17">
+        <v>2.6000000000000001E-8</v>
+      </c>
+      <c r="BI14" s="17">
+        <v>2.6000000000000001E-8</v>
+      </c>
     </row>
-    <row r="15" spans="1:58" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:61" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -13022,8 +14031,23 @@
       <c r="BD15" s="7">
         <v>1026</v>
       </c>
+      <c r="BE15" s="7">
+        <v>1026</v>
+      </c>
+      <c r="BF15" s="7">
+        <v>1026</v>
+      </c>
+      <c r="BG15" s="7">
+        <v>1026</v>
+      </c>
+      <c r="BH15" s="7">
+        <v>1026</v>
+      </c>
+      <c r="BI15" s="7">
+        <v>1026</v>
+      </c>
     </row>
-    <row r="16" spans="1:58" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:61" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -13192,8 +14216,23 @@
       <c r="BD16" s="7">
         <v>96</v>
       </c>
+      <c r="BE16" s="7">
+        <v>96</v>
+      </c>
+      <c r="BF16" s="7">
+        <v>96</v>
+      </c>
+      <c r="BG16" s="7">
+        <v>96</v>
+      </c>
+      <c r="BH16" s="7">
+        <v>96</v>
+      </c>
+      <c r="BI16" s="7">
+        <v>96</v>
+      </c>
     </row>
-    <row r="17" spans="1:56" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:61" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>15</v>
       </c>
@@ -13362,8 +14401,23 @@
       <c r="BD17" s="7">
         <v>2439</v>
       </c>
+      <c r="BE17" s="7">
+        <v>2439</v>
+      </c>
+      <c r="BF17" s="7">
+        <v>2439</v>
+      </c>
+      <c r="BG17" s="7">
+        <v>2439</v>
+      </c>
+      <c r="BH17" s="7">
+        <v>2439</v>
+      </c>
+      <c r="BI17" s="7">
+        <v>2439</v>
+      </c>
     </row>
-    <row r="18" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:61" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>16</v>
       </c>
@@ -13532,8 +14586,23 @@
       <c r="BD18" s="7">
         <v>0</v>
       </c>
+      <c r="BE18" s="7">
+        <v>0</v>
+      </c>
+      <c r="BF18" s="7">
+        <v>0</v>
+      </c>
+      <c r="BG18" s="7">
+        <v>0</v>
+      </c>
+      <c r="BH18" s="7">
+        <v>0</v>
+      </c>
+      <c r="BI18" s="7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:61" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>17</v>
       </c>
@@ -13702,8 +14771,23 @@
       <c r="BD19" s="10">
         <v>4300</v>
       </c>
+      <c r="BE19" s="10">
+        <v>4300</v>
+      </c>
+      <c r="BF19" s="10">
+        <v>4300</v>
+      </c>
+      <c r="BG19" s="10">
+        <v>4300</v>
+      </c>
+      <c r="BH19" s="10">
+        <v>4300</v>
+      </c>
+      <c r="BI19" s="10">
+        <v>4300</v>
+      </c>
     </row>
-    <row r="20" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:61" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>18</v>
       </c>
@@ -13872,8 +14956,23 @@
       <c r="BD20" s="10">
         <v>9320</v>
       </c>
+      <c r="BE20" s="10">
+        <v>9320</v>
+      </c>
+      <c r="BF20" s="10">
+        <v>9320</v>
+      </c>
+      <c r="BG20" s="10">
+        <v>9320</v>
+      </c>
+      <c r="BH20" s="10">
+        <v>9320</v>
+      </c>
+      <c r="BI20" s="10">
+        <v>9320</v>
+      </c>
     </row>
-    <row r="21" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:61" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>19</v>
       </c>
@@ -14042,8 +15141,23 @@
       <c r="BD21" s="10">
         <v>13860</v>
       </c>
+      <c r="BE21" s="10">
+        <v>13860</v>
+      </c>
+      <c r="BF21" s="10">
+        <v>13860</v>
+      </c>
+      <c r="BG21" s="10">
+        <v>13860</v>
+      </c>
+      <c r="BH21" s="10">
+        <v>13860</v>
+      </c>
+      <c r="BI21" s="10">
+        <v>13860</v>
+      </c>
     </row>
-    <row r="22" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:61" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>20</v>
       </c>
@@ -14212,8 +15326,23 @@
       <c r="BD22" s="10">
         <v>21660</v>
       </c>
+      <c r="BE22" s="10">
+        <v>21660</v>
+      </c>
+      <c r="BF22" s="10">
+        <v>21660</v>
+      </c>
+      <c r="BG22" s="10">
+        <v>21660</v>
+      </c>
+      <c r="BH22" s="10">
+        <v>21660</v>
+      </c>
+      <c r="BI22" s="10">
+        <v>21660</v>
+      </c>
     </row>
-    <row r="23" spans="1:56" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:61" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>21</v>
       </c>
@@ -14382,8 +15511,23 @@
       <c r="BD23" s="10">
         <v>25000</v>
       </c>
+      <c r="BE23" s="10">
+        <v>25000</v>
+      </c>
+      <c r="BF23" s="10">
+        <v>25000</v>
+      </c>
+      <c r="BG23" s="10">
+        <v>25000</v>
+      </c>
+      <c r="BH23" s="10">
+        <v>25000</v>
+      </c>
+      <c r="BI23" s="10">
+        <v>25000</v>
+      </c>
     </row>
-    <row r="24" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>22</v>
       </c>
@@ -14552,8 +15696,23 @@
       <c r="BD24" s="7">
         <v>2972</v>
       </c>
+      <c r="BE24" s="7">
+        <v>2972</v>
+      </c>
+      <c r="BF24" s="7">
+        <v>2972</v>
+      </c>
+      <c r="BG24" s="7">
+        <v>2972</v>
+      </c>
+      <c r="BH24" s="7">
+        <v>2972</v>
+      </c>
+      <c r="BI24" s="7">
+        <v>2972</v>
+      </c>
     </row>
-    <row r="25" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>23</v>
       </c>
@@ -14722,8 +15881,23 @@
       <c r="BD25" s="7">
         <v>3</v>
       </c>
+      <c r="BE25" s="7">
+        <v>3</v>
+      </c>
+      <c r="BF25" s="7">
+        <v>3</v>
+      </c>
+      <c r="BG25" s="7">
+        <v>3</v>
+      </c>
+      <c r="BH25" s="7">
+        <v>3</v>
+      </c>
+      <c r="BI25" s="7">
+        <v>3</v>
+      </c>
     </row>
-    <row r="26" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>24</v>
       </c>
@@ -14892,8 +16066,23 @@
       <c r="BD26" s="7">
         <v>1</v>
       </c>
+      <c r="BE26" s="7">
+        <v>1</v>
+      </c>
+      <c r="BF26" s="7">
+        <v>1</v>
+      </c>
+      <c r="BG26" s="7">
+        <v>1</v>
+      </c>
+      <c r="BH26" s="7">
+        <v>1</v>
+      </c>
+      <c r="BI26" s="7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>25</v>
       </c>
@@ -15062,8 +16251,23 @@
       <c r="BD27" s="14">
         <v>0</v>
       </c>
+      <c r="BE27" s="14">
+        <v>0</v>
+      </c>
+      <c r="BF27" s="14">
+        <v>0</v>
+      </c>
+      <c r="BG27" s="14">
+        <v>0</v>
+      </c>
+      <c r="BH27" s="14">
+        <v>0</v>
+      </c>
+      <c r="BI27" s="14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>26</v>
       </c>
@@ -15232,8 +16436,23 @@
       <c r="BD28" s="7">
         <v>365</v>
       </c>
+      <c r="BE28" s="7">
+        <v>365</v>
+      </c>
+      <c r="BF28" s="7">
+        <v>365</v>
+      </c>
+      <c r="BG28" s="7">
+        <v>365</v>
+      </c>
+      <c r="BH28" s="7">
+        <v>365</v>
+      </c>
+      <c r="BI28" s="7">
+        <v>365</v>
+      </c>
     </row>
-    <row r="29" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>27</v>
       </c>
@@ -15402,8 +16621,23 @@
       <c r="BD29" s="14">
         <v>580</v>
       </c>
+      <c r="BE29" s="14">
+        <v>580</v>
+      </c>
+      <c r="BF29" s="14">
+        <v>580</v>
+      </c>
+      <c r="BG29" s="14">
+        <v>580</v>
+      </c>
+      <c r="BH29" s="14">
+        <v>580</v>
+      </c>
+      <c r="BI29" s="14">
+        <v>580</v>
+      </c>
     </row>
-    <row r="30" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>28</v>
       </c>
@@ -15572,8 +16806,23 @@
       <c r="BD30" s="14">
         <v>0</v>
       </c>
+      <c r="BE30" s="14">
+        <v>0</v>
+      </c>
+      <c r="BF30" s="14">
+        <v>0</v>
+      </c>
+      <c r="BG30" s="14">
+        <v>0</v>
+      </c>
+      <c r="BH30" s="14">
+        <v>0</v>
+      </c>
+      <c r="BI30" s="14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>29</v>
       </c>
@@ -15742,8 +16991,23 @@
       <c r="BD31" s="14">
         <v>0</v>
       </c>
+      <c r="BE31" s="14">
+        <v>0</v>
+      </c>
+      <c r="BF31" s="14">
+        <v>0</v>
+      </c>
+      <c r="BG31" s="14">
+        <v>0</v>
+      </c>
+      <c r="BH31" s="14">
+        <v>0</v>
+      </c>
+      <c r="BI31" s="14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>30</v>
       </c>
@@ -15912,8 +17176,23 @@
       <c r="BD32" s="14">
         <v>0</v>
       </c>
+      <c r="BE32" s="14">
+        <v>0</v>
+      </c>
+      <c r="BF32" s="14">
+        <v>0</v>
+      </c>
+      <c r="BG32" s="14">
+        <v>0</v>
+      </c>
+      <c r="BH32" s="14">
+        <v>0</v>
+      </c>
+      <c r="BI32" s="14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>31</v>
       </c>
@@ -16082,8 +17361,23 @@
       <c r="BD33" s="14">
         <v>0</v>
       </c>
+      <c r="BE33" s="14">
+        <v>0</v>
+      </c>
+      <c r="BF33" s="14">
+        <v>0</v>
+      </c>
+      <c r="BG33" s="14">
+        <v>0</v>
+      </c>
+      <c r="BH33" s="14">
+        <v>0</v>
+      </c>
+      <c r="BI33" s="14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>32</v>
       </c>
@@ -16252,8 +17546,23 @@
       <c r="BD34" s="14">
         <v>7420</v>
       </c>
+      <c r="BE34" s="14">
+        <v>7420</v>
+      </c>
+      <c r="BF34" s="14">
+        <v>7420</v>
+      </c>
+      <c r="BG34" s="14">
+        <v>7420</v>
+      </c>
+      <c r="BH34" s="14">
+        <v>7420</v>
+      </c>
+      <c r="BI34" s="14">
+        <v>7420</v>
+      </c>
     </row>
-    <row r="35" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>33</v>
       </c>
@@ -16422,8 +17731,23 @@
       <c r="BD35" s="7">
         <v>6025</v>
       </c>
+      <c r="BE35" s="7">
+        <v>6025</v>
+      </c>
+      <c r="BF35" s="7">
+        <v>6025</v>
+      </c>
+      <c r="BG35" s="7">
+        <v>6025</v>
+      </c>
+      <c r="BH35" s="7">
+        <v>6025</v>
+      </c>
+      <c r="BI35" s="7">
+        <v>6025</v>
+      </c>
     </row>
-    <row r="36" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>34</v>
       </c>
@@ -16592,8 +17916,23 @@
       <c r="BD36" s="7">
         <v>178</v>
       </c>
+      <c r="BE36" s="7">
+        <v>178</v>
+      </c>
+      <c r="BF36" s="7">
+        <v>178</v>
+      </c>
+      <c r="BG36" s="7">
+        <v>178</v>
+      </c>
+      <c r="BH36" s="7">
+        <v>178</v>
+      </c>
+      <c r="BI36" s="7">
+        <v>178</v>
+      </c>
     </row>
-    <row r="37" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>35</v>
       </c>
@@ -16762,8 +18101,23 @@
       <c r="BD37" s="7" t="s">
         <v>193</v>
       </c>
+      <c r="BE37" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BF37" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BG37" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BH37" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="BI37" s="7" t="s">
+        <v>193</v>
+      </c>
     </row>
-    <row r="38" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>36</v>
       </c>
@@ -16932,8 +18286,23 @@
       <c r="BD38" s="7">
         <v>67397790</v>
       </c>
+      <c r="BE38" s="7">
+        <v>67397790</v>
+      </c>
+      <c r="BF38" s="7">
+        <v>67397790</v>
+      </c>
+      <c r="BG38" s="7">
+        <v>67397790</v>
+      </c>
+      <c r="BH38" s="7">
+        <v>67397790</v>
+      </c>
+      <c r="BI38" s="7">
+        <v>67397790</v>
+      </c>
     </row>
-    <row r="39" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>37</v>
       </c>
@@ -17102,8 +18471,23 @@
       <c r="BD39" s="7">
         <v>54644647</v>
       </c>
+      <c r="BE39" s="7">
+        <v>54644647</v>
+      </c>
+      <c r="BF39" s="7">
+        <v>54644647</v>
+      </c>
+      <c r="BG39" s="7">
+        <v>54644647</v>
+      </c>
+      <c r="BH39" s="7">
+        <v>54644647</v>
+      </c>
+      <c r="BI39" s="7">
+        <v>54644647</v>
+      </c>
     </row>
-    <row r="40" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>38</v>
       </c>
@@ -17272,8 +18656,23 @@
       <c r="BD40" s="7">
         <v>88722733</v>
       </c>
+      <c r="BE40" s="7">
+        <v>88722733</v>
+      </c>
+      <c r="BF40" s="7">
+        <v>88722733</v>
+      </c>
+      <c r="BG40" s="7">
+        <v>88722733</v>
+      </c>
+      <c r="BH40" s="7">
+        <v>88722733</v>
+      </c>
+      <c r="BI40" s="7">
+        <v>88722733</v>
+      </c>
     </row>
-    <row r="41" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>39</v>
       </c>
@@ -17442,8 +18841,23 @@
       <c r="BD41" s="7">
         <v>92846918</v>
       </c>
+      <c r="BE41" s="7">
+        <v>92846918</v>
+      </c>
+      <c r="BF41" s="7">
+        <v>92846918</v>
+      </c>
+      <c r="BG41" s="7">
+        <v>92846918</v>
+      </c>
+      <c r="BH41" s="7">
+        <v>92846918</v>
+      </c>
+      <c r="BI41" s="7">
+        <v>92846918</v>
+      </c>
     </row>
-    <row r="42" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>40</v>
       </c>
@@ -17612,8 +19026,23 @@
       <c r="BD42" s="7">
         <v>100533789</v>
       </c>
+      <c r="BE42" s="7">
+        <v>100533789</v>
+      </c>
+      <c r="BF42" s="7">
+        <v>100533789</v>
+      </c>
+      <c r="BG42" s="7">
+        <v>100533789</v>
+      </c>
+      <c r="BH42" s="7">
+        <v>100533789</v>
+      </c>
+      <c r="BI42" s="7">
+        <v>100533789</v>
+      </c>
     </row>
-    <row r="43" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>41</v>
       </c>
@@ -17782,8 +19211,23 @@
       <c r="BD43" s="14">
         <v>0.998</v>
       </c>
+      <c r="BE43" s="14">
+        <v>0.998</v>
+      </c>
+      <c r="BF43" s="14">
+        <v>0.998</v>
+      </c>
+      <c r="BG43" s="14">
+        <v>0.998</v>
+      </c>
+      <c r="BH43" s="14">
+        <v>0.998</v>
+      </c>
+      <c r="BI43" s="14">
+        <v>0.998</v>
+      </c>
     </row>
-    <row r="44" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>42</v>
       </c>
@@ -17952,8 +19396,23 @@
       <c r="BD44" s="14">
         <v>-10</v>
       </c>
+      <c r="BE44" s="14">
+        <v>-10</v>
+      </c>
+      <c r="BF44" s="14">
+        <v>-10</v>
+      </c>
+      <c r="BG44" s="14">
+        <v>-10</v>
+      </c>
+      <c r="BH44" s="14">
+        <v>-10</v>
+      </c>
+      <c r="BI44" s="14">
+        <v>-10</v>
+      </c>
     </row>
-    <row r="45" spans="1:56" s="10" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:61" s="10" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>43</v>
       </c>
@@ -18122,8 +19581,23 @@
       <c r="BD45" s="7">
         <v>1732</v>
       </c>
+      <c r="BE45" s="7">
+        <v>1732</v>
+      </c>
+      <c r="BF45" s="7">
+        <v>1732</v>
+      </c>
+      <c r="BG45" s="7">
+        <v>1732</v>
+      </c>
+      <c r="BH45" s="7">
+        <v>1732</v>
+      </c>
+      <c r="BI45" s="7">
+        <v>1732</v>
+      </c>
     </row>
-    <row r="46" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>44</v>
       </c>
@@ -18292,8 +19766,23 @@
       <c r="BD46" s="7">
         <v>250</v>
       </c>
+      <c r="BE46" s="7">
+        <v>250</v>
+      </c>
+      <c r="BF46" s="7">
+        <v>250</v>
+      </c>
+      <c r="BG46" s="7">
+        <v>250</v>
+      </c>
+      <c r="BH46" s="7">
+        <v>250</v>
+      </c>
+      <c r="BI46" s="7">
+        <v>250</v>
+      </c>
     </row>
-    <row r="47" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>45</v>
       </c>
@@ -18462,8 +19951,23 @@
       <c r="BD47" s="7">
         <v>0</v>
       </c>
+      <c r="BE47" s="7">
+        <v>0</v>
+      </c>
+      <c r="BF47" s="7">
+        <v>0</v>
+      </c>
+      <c r="BG47" s="7">
+        <v>0</v>
+      </c>
+      <c r="BH47" s="7">
+        <v>0</v>
+      </c>
+      <c r="BI47" s="7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>46</v>
       </c>
@@ -18632,8 +20136,23 @@
       <c r="BD48" s="7">
         <v>64</v>
       </c>
+      <c r="BE48" s="7">
+        <v>64</v>
+      </c>
+      <c r="BF48" s="7">
+        <v>64</v>
+      </c>
+      <c r="BG48" s="7">
+        <v>64</v>
+      </c>
+      <c r="BH48" s="7">
+        <v>64</v>
+      </c>
+      <c r="BI48" s="7">
+        <v>64</v>
+      </c>
     </row>
-    <row r="49" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <v>47</v>
       </c>
@@ -18802,8 +20321,23 @@
       <c r="BD49" s="7">
         <v>256</v>
       </c>
+      <c r="BE49" s="7">
+        <v>256</v>
+      </c>
+      <c r="BF49" s="7">
+        <v>256</v>
+      </c>
+      <c r="BG49" s="7">
+        <v>256</v>
+      </c>
+      <c r="BH49" s="7">
+        <v>256</v>
+      </c>
+      <c r="BI49" s="7">
+        <v>256</v>
+      </c>
     </row>
-    <row r="50" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>48</v>
       </c>
@@ -18972,8 +20506,23 @@
       <c r="BD50" s="7">
         <v>0</v>
       </c>
+      <c r="BE50" s="7">
+        <v>0</v>
+      </c>
+      <c r="BF50" s="7">
+        <v>0</v>
+      </c>
+      <c r="BG50" s="7">
+        <v>0</v>
+      </c>
+      <c r="BH50" s="7">
+        <v>0</v>
+      </c>
+      <c r="BI50" s="7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="51" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>49</v>
       </c>
@@ -19142,8 +20691,23 @@
       <c r="BD51" s="7">
         <v>64</v>
       </c>
+      <c r="BE51" s="7">
+        <v>64</v>
+      </c>
+      <c r="BF51" s="7">
+        <v>64</v>
+      </c>
+      <c r="BG51" s="7">
+        <v>64</v>
+      </c>
+      <c r="BH51" s="7">
+        <v>64</v>
+      </c>
+      <c r="BI51" s="7">
+        <v>64</v>
+      </c>
     </row>
-    <row r="52" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>50</v>
       </c>
@@ -19312,8 +20876,23 @@
       <c r="BD52" s="7">
         <v>56</v>
       </c>
+      <c r="BE52" s="7">
+        <v>56</v>
+      </c>
+      <c r="BF52" s="7">
+        <v>56</v>
+      </c>
+      <c r="BG52" s="7">
+        <v>56</v>
+      </c>
+      <c r="BH52" s="7">
+        <v>56</v>
+      </c>
+      <c r="BI52" s="7">
+        <v>56</v>
+      </c>
     </row>
-    <row r="53" spans="1:56" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:61" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>51</v>
       </c>
@@ -19482,8 +21061,23 @@
       <c r="BD53" s="7">
         <v>2226</v>
       </c>
+      <c r="BE53" s="7">
+        <v>2226</v>
+      </c>
+      <c r="BF53" s="7">
+        <v>2226</v>
+      </c>
+      <c r="BG53" s="7">
+        <v>2226</v>
+      </c>
+      <c r="BH53" s="7">
+        <v>2226</v>
+      </c>
+      <c r="BI53" s="7">
+        <v>2226</v>
+      </c>
     </row>
-    <row r="54" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
         <v>52</v>
       </c>
@@ -19509,18 +21103,18 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55:C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.3984375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.3984375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="4" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="19.19921875" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -20241,7 +21835,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="20">
-        <f t="shared" ref="A41:A54" si="2">+B41-693960</f>
+        <f t="shared" ref="A41:A59" si="2">+B41-693960</f>
         <v>41800</v>
       </c>
       <c r="B41" s="4">
@@ -20492,7 +22086,94 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C55" s="22"/>
+      <c r="A55" s="5">
+        <f t="shared" si="2"/>
+        <v>42646</v>
+      </c>
+      <c r="B55" s="4">
+        <v>736606</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="D55" t="s">
+        <v>208</v>
+      </c>
+      <c r="E55">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="5">
+        <f t="shared" si="2"/>
+        <v>42661</v>
+      </c>
+      <c r="B56" s="4">
+        <v>736621</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="D56" t="s">
+        <v>208</v>
+      </c>
+      <c r="E56">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="5">
+        <f t="shared" si="2"/>
+        <v>42705</v>
+      </c>
+      <c r="B57" s="4">
+        <v>736665</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="D57" t="s">
+        <v>208</v>
+      </c>
+      <c r="E57">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="5">
+        <f t="shared" si="2"/>
+        <v>42709</v>
+      </c>
+      <c r="B58" s="4">
+        <v>736669</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="D58" t="s">
+        <v>208</v>
+      </c>
+      <c r="E58">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="5">
+        <f t="shared" si="2"/>
+        <v>42710</v>
+      </c>
+      <c r="B59" s="4">
+        <v>736670</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="D59" t="s">
+        <v>208</v>
+      </c>
+      <c r="E59">
+        <v>350</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -20507,20 +22188,20 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja3" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:E98"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.3984375" style="21" customWidth="1"/>
-    <col min="2" max="2" width="43.796875" style="22" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="21" customWidth="1"/>
+    <col min="2" max="2" width="43.83203125" style="22" customWidth="1"/>
     <col min="3" max="3" width="12" style="7" customWidth="1"/>
     <col min="4" max="4" width="17" style="7" customWidth="1"/>
-    <col min="5" max="5" width="18.59765625" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="11.3984375" style="7"/>
+    <col min="5" max="5" width="18.5" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="105" x14ac:dyDescent="0.2">
@@ -20555,7 +22236,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="21">
         <v>40349</v>
       </c>
@@ -20682,7 +22363,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="90" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.2">
       <c r="A16" s="21">
         <v>40646</v>
       </c>
@@ -20690,7 +22371,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="21">
         <v>40665</v>
       </c>
@@ -20698,7 +22379,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A18" s="21">
         <v>40667</v>
       </c>
@@ -20733,7 +22414,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="21">
         <v>40696</v>
       </c>
@@ -21013,7 +22694,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="24">
         <v>41225</v>
       </c>
@@ -21072,7 +22753,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="21">
         <v>41354</v>
       </c>
@@ -21124,7 +22805,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="21">
         <v>41519</v>
       </c>
@@ -21156,7 +22837,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="26">
         <v>41682</v>
       </c>
@@ -21276,7 +22957,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="82" spans="1:5" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="28">
         <v>41974</v>
       </c>
@@ -21427,6 +23108,46 @@
       </c>
       <c r="B98" s="22" t="s">
         <v>217</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="21">
+        <v>42646</v>
+      </c>
+      <c r="B99" s="22" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="21">
+        <v>42661</v>
+      </c>
+      <c r="B100" s="22" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="21">
+        <v>42705</v>
+      </c>
+      <c r="B101" s="22" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="21">
+        <v>42709</v>
+      </c>
+      <c r="B102" s="22" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="21">
+        <v>42710</v>
+      </c>
+      <c r="B103" s="22" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -22701,9 +24422,9 @@
         <f>AND(icf.157!AA12,"AAAAAG9/uzc=")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BE2">
+      <c r="BE2" t="str">
         <f>IF(icf.157!13:13,"AAAAAG9/uzg=",0)</f>
-        <v>0</v>
+        <v>AAAAAG9/uzg=</v>
       </c>
       <c r="BF2" t="e">
         <f>AND(icf.157!A13,"AAAAAG9/uzk=")</f>
@@ -23743,9 +25464,9 @@
         <f>AND(icf.157!AA22,"AAAAAHuxazs=")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BI3">
+      <c r="BI3" t="str">
         <f>IF(icf.157!23:23,"AAAAAHuxazw=",0)</f>
-        <v>0</v>
+        <v>AAAAAHuxazw=</v>
       </c>
       <c r="BJ3" t="e">
         <f>AND(icf.157!A23,"AAAAAHuxaz0=")</f>
@@ -28154,12 +29875,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.796875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="29.19921875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.3984375" customWidth="1"/>
-    <col min="5" max="23" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.3984375" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="23" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>